<commit_message>
Update zero prandtl number
</commit_message>
<xml_diff>
--- a/dedalus_case.xlsx
+++ b/dedalus_case.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nutstore\Nutstore\Workspace\dedalus_main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59619E5A-E889-4E28-946D-50BC098FCAC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D498A522-D4ED-4D37-82F2-985088D2B04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="49">
   <si>
     <t>slurm_num</t>
   </si>
@@ -174,6 +174,15 @@
   </si>
   <si>
     <t>infinity</t>
+  </si>
+  <si>
+    <t>nx_trunc_num=1, nz_trunc_num=2</t>
+  </si>
+  <si>
+    <t>nx_trunc_num=1, nz_trunc_num=2, with A_noise=0.01</t>
+  </si>
+  <si>
+    <t>nx_trunc_num=1, nz_trunc_num=1000</t>
   </si>
 </sst>
 </file>
@@ -547,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P59"/>
+  <dimension ref="A1:P74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2314,6 +2323,417 @@
         <v>100000000</v>
       </c>
     </row>
+    <row r="61" spans="1:14">
+      <c r="A61" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14">
+      <c r="A62" s="1">
+        <v>14965608</v>
+      </c>
+      <c r="B62">
+        <v>30000</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>128</v>
+      </c>
+      <c r="G62">
+        <v>128</v>
+      </c>
+      <c r="H62">
+        <v>10</v>
+      </c>
+      <c r="I62">
+        <v>10</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="L62">
+        <v>10</v>
+      </c>
+      <c r="M62">
+        <v>0.01</v>
+      </c>
+      <c r="N62" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="A63" s="1">
+        <v>14965609</v>
+      </c>
+      <c r="B63">
+        <v>40000</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>13</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>128</v>
+      </c>
+      <c r="G63">
+        <v>128</v>
+      </c>
+      <c r="H63">
+        <v>10</v>
+      </c>
+      <c r="I63">
+        <v>10</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="L63">
+        <v>10</v>
+      </c>
+      <c r="M63">
+        <v>0.01</v>
+      </c>
+      <c r="N63" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="A64" s="1">
+        <v>14965611</v>
+      </c>
+      <c r="B64">
+        <v>60000</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
+        <v>13</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>128</v>
+      </c>
+      <c r="G64">
+        <v>128</v>
+      </c>
+      <c r="H64">
+        <v>10</v>
+      </c>
+      <c r="I64">
+        <v>10</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="L64">
+        <v>10</v>
+      </c>
+      <c r="M64">
+        <v>0.01</v>
+      </c>
+      <c r="N64" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
+      <c r="A66" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14">
+      <c r="A67" s="1">
+        <v>14965912</v>
+      </c>
+      <c r="B67">
+        <v>30000</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67" t="s">
+        <v>13</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67">
+        <v>128</v>
+      </c>
+      <c r="G67">
+        <v>128</v>
+      </c>
+      <c r="H67">
+        <v>10</v>
+      </c>
+      <c r="I67">
+        <v>10</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="L67">
+        <v>10</v>
+      </c>
+      <c r="M67">
+        <v>0.01</v>
+      </c>
+      <c r="N67" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14">
+      <c r="A68" s="1">
+        <v>14965914</v>
+      </c>
+      <c r="B68">
+        <v>40000</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68" t="s">
+        <v>13</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>128</v>
+      </c>
+      <c r="G68">
+        <v>128</v>
+      </c>
+      <c r="H68">
+        <v>10</v>
+      </c>
+      <c r="I68">
+        <v>10</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+      <c r="K68" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="L68">
+        <v>10</v>
+      </c>
+      <c r="M68">
+        <v>0.01</v>
+      </c>
+      <c r="N68" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14">
+      <c r="A69" s="1">
+        <v>14965915</v>
+      </c>
+      <c r="B69">
+        <v>60000</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69" t="s">
+        <v>13</v>
+      </c>
+      <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69">
+        <v>128</v>
+      </c>
+      <c r="G69">
+        <v>128</v>
+      </c>
+      <c r="H69">
+        <v>10</v>
+      </c>
+      <c r="I69">
+        <v>10</v>
+      </c>
+      <c r="J69">
+        <v>0</v>
+      </c>
+      <c r="K69" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="L69">
+        <v>10</v>
+      </c>
+      <c r="M69">
+        <v>0.01</v>
+      </c>
+      <c r="N69" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14">
+      <c r="A71" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14">
+      <c r="A72" s="1">
+        <v>14965918</v>
+      </c>
+      <c r="B72">
+        <v>30000</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72" t="s">
+        <v>13</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <v>128</v>
+      </c>
+      <c r="G72">
+        <v>128</v>
+      </c>
+      <c r="H72">
+        <v>10</v>
+      </c>
+      <c r="I72">
+        <v>10</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="L72">
+        <v>10</v>
+      </c>
+      <c r="M72">
+        <v>0.01</v>
+      </c>
+      <c r="N72" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14">
+      <c r="A73" s="1">
+        <v>14965919</v>
+      </c>
+      <c r="B73">
+        <v>40000</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73" t="s">
+        <v>13</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73">
+        <v>128</v>
+      </c>
+      <c r="G73">
+        <v>128</v>
+      </c>
+      <c r="H73">
+        <v>10</v>
+      </c>
+      <c r="I73">
+        <v>10</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="L73">
+        <v>10</v>
+      </c>
+      <c r="M73">
+        <v>0.01</v>
+      </c>
+      <c r="N73" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14">
+      <c r="A74" s="1">
+        <v>14965920</v>
+      </c>
+      <c r="B74">
+        <v>60000</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74" t="s">
+        <v>13</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74">
+        <v>128</v>
+      </c>
+      <c r="G74">
+        <v>128</v>
+      </c>
+      <c r="H74">
+        <v>10</v>
+      </c>
+      <c r="I74">
+        <v>10</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+      <c r="K74" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="L74">
+        <v>10</v>
+      </c>
+      <c r="M74">
+        <v>0.01</v>
+      </c>
+      <c r="N74" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update the time storage
</commit_message>
<xml_diff>
--- a/dedalus_case.xlsx
+++ b/dedalus_case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nutstore\Nutstore\Workspace\dedalus_main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2640D6C-211C-4200-8F54-E74D44933702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418EB9E3-F762-4036-88BE-33F0E6C661DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RBC flux" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1522" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1527" uniqueCount="234">
   <si>
     <t>slurm_num</t>
   </si>
@@ -742,6 +742,9 @@
   <si>
     <t>Need to make shear stronger and no_phase_step=10</t>
   </si>
+  <si>
+    <t>2pi/18</t>
+  </si>
 </sst>
 </file>
 
@@ -24200,15 +24203,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFDB63EE-010E-4366-8142-3356469E97C6}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:14">
       <c r="C1" s="19" t="s">
         <v>206</v>
       </c>
@@ -24233,13 +24236,58 @@
       <c r="J1" s="19" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>228</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
+      </c>
+      <c r="C2">
+        <v>100000</v>
+      </c>
+      <c r="D2">
+        <v>40</v>
+      </c>
+      <c r="E2">
+        <v>0.01</v>
+      </c>
+      <c r="F2">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>233</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>128</v>
+      </c>
+      <c r="J2">
+        <v>128</v>
+      </c>
+      <c r="K2">
+        <v>1E-3</v>
+      </c>
+      <c r="L2">
+        <v>0.3</v>
+      </c>
+      <c r="M2">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -24251,8 +24299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D76C9478-386D-445B-8B12-05AF01279C9C}">
   <dimension ref="A3:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+    <sheetView topLeftCell="C39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Update sub flow is wrong
</commit_message>
<xml_diff>
--- a/dedalus_case.xlsx
+++ b/dedalus_case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nutstore\Nutstore\Workspace\dedalus_main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BE09A2-E075-448F-B84C-8E56DA570DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB5150FA-A1BC-4DFA-9EC8-5879BCF5E5F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RBC flux" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1559" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="255">
   <si>
     <t>slurm_num</t>
   </si>
@@ -793,6 +793,21 @@
   <si>
     <t>conduction</t>
   </si>
+  <si>
+    <t>Update 2023/06/16 generate phase shifted X2 solution</t>
+  </si>
+  <si>
+    <t>2 wave localized</t>
+  </si>
+  <si>
+    <t>with new parameter initial_phase=pi/2</t>
+  </si>
+  <si>
+    <t>Test beta=10^4, initial value as random variable</t>
+  </si>
+  <si>
+    <t>elevator mode + A_noise=0.1</t>
+  </si>
 </sst>
 </file>
 
@@ -1243,22 +1258,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S385"/>
+  <dimension ref="A1:S392"/>
   <sheetViews>
-    <sheetView topLeftCell="A129" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C165" sqref="C165"/>
+    <sheetView tabSelected="1" topLeftCell="A387" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B393" sqref="B393"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.453125" customWidth="1"/>
-    <col min="2" max="2" width="21.54296875" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" customWidth="1"/>
-    <col min="10" max="10" width="11.7265625" customWidth="1"/>
-    <col min="11" max="11" width="15.54296875" customWidth="1"/>
-    <col min="12" max="12" width="14.81640625" customWidth="1"/>
-    <col min="13" max="13" width="14.54296875" customWidth="1"/>
-    <col min="16" max="16" width="12.7265625" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15">
@@ -2433,7 +2448,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="24" customFormat="1" ht="18.5">
+    <row r="38" spans="1:16" s="24" customFormat="1" ht="18.75">
       <c r="B38" s="51">
         <v>14673046</v>
       </c>
@@ -2508,7 +2523,7 @@
       </c>
       <c r="C43" s="2"/>
     </row>
-    <row r="44" spans="1:16" ht="18.5">
+    <row r="44" spans="1:16" ht="18.75">
       <c r="B44" s="3">
         <v>14541125</v>
       </c>
@@ -2555,7 +2570,7 @@
         <v>12.0533</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="18.5">
+    <row r="45" spans="1:16" ht="18.75">
       <c r="B45" s="3">
         <v>14541126</v>
       </c>
@@ -2602,7 +2617,7 @@
         <v>12.0533</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="18.5">
+    <row r="46" spans="1:16" ht="18.75">
       <c r="B46" s="3">
         <v>14541127</v>
       </c>
@@ -2649,7 +2664,7 @@
         <v>12.0533</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="18.5">
+    <row r="47" spans="1:16" ht="18.75">
       <c r="B47" s="3">
         <v>14541128</v>
       </c>
@@ -2786,7 +2801,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="56" spans="2:16" ht="18.5">
+    <row r="56" spans="2:16" ht="18.75">
       <c r="B56" s="3">
         <v>14673046</v>
       </c>
@@ -2830,7 +2845,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="2:16" ht="18.5">
+    <row r="57" spans="2:16" ht="18.75">
       <c r="B57" s="3">
         <v>14673047</v>
       </c>
@@ -2874,7 +2889,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="2:16" ht="18.5">
+    <row r="58" spans="2:16" ht="18.75">
       <c r="B58" s="3">
         <v>14768718</v>
       </c>
@@ -2915,7 +2930,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="59" spans="2:16" ht="18.5">
+    <row r="59" spans="2:16" ht="18.75">
       <c r="B59" s="3">
         <v>14680791</v>
       </c>
@@ -2959,7 +2974,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="2:16" ht="18.5">
+    <row r="60" spans="2:16" ht="18.75">
       <c r="B60" s="3">
         <v>14741869</v>
       </c>
@@ -3003,7 +3018,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="2:16" ht="18.5">
+    <row r="61" spans="2:16" ht="18.75">
       <c r="B61" s="3">
         <v>14673849</v>
       </c>
@@ -3044,7 +3059,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="62" spans="2:16" ht="18.5">
+    <row r="62" spans="2:16" ht="18.75">
       <c r="B62" s="3">
         <v>14673048</v>
       </c>
@@ -3088,7 +3103,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="2:16" ht="18.5">
+    <row r="63" spans="2:16" ht="18.75">
       <c r="B63" s="3">
         <v>14673049</v>
       </c>
@@ -3222,7 +3237,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="2:15" ht="18.5">
+    <row r="68" spans="2:15" ht="18.75">
       <c r="B68" s="3">
         <v>14680810</v>
       </c>
@@ -3266,7 +3281,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="2:15" ht="18.5">
+    <row r="69" spans="2:15" ht="18.75">
       <c r="B69" s="3">
         <v>14672941</v>
       </c>
@@ -3310,7 +3325,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="2:15" ht="18.5">
+    <row r="70" spans="2:15" ht="18.75">
       <c r="B70" s="3">
         <v>14672942</v>
       </c>
@@ -3354,7 +3369,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="2:15" ht="18.5">
+    <row r="71" spans="2:15" ht="18.75">
       <c r="B71" s="3">
         <v>14672943</v>
       </c>
@@ -3398,7 +3413,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="2:15" ht="18.5">
+    <row r="72" spans="2:15" ht="18.75">
       <c r="B72" s="3">
         <v>14672940</v>
       </c>
@@ -3442,7 +3457,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="2:15" ht="17.5">
+    <row r="73" spans="2:15" ht="18">
       <c r="B73" s="4">
         <v>14671572</v>
       </c>
@@ -3486,7 +3501,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="2:15" ht="17.5">
+    <row r="74" spans="2:15" ht="18">
       <c r="B74" s="4">
         <v>14680814</v>
       </c>
@@ -3530,7 +3545,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="2:15" ht="17.5">
+    <row r="75" spans="2:15" ht="18">
       <c r="B75" s="4">
         <v>14671573</v>
       </c>
@@ -15511,7 +15526,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="385" spans="3:12">
+    <row r="385" spans="1:14">
       <c r="C385" s="2">
         <v>100000000</v>
       </c>
@@ -15541,6 +15556,140 @@
       </c>
       <c r="L385" s="2">
         <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="389" spans="1:14">
+      <c r="A389" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="390" spans="1:14">
+      <c r="A390" t="s">
+        <v>254</v>
+      </c>
+      <c r="B390">
+        <v>15565217</v>
+      </c>
+      <c r="C390" s="2">
+        <v>30000</v>
+      </c>
+      <c r="D390" s="8">
+        <v>1</v>
+      </c>
+      <c r="E390" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F390" s="8">
+        <v>1</v>
+      </c>
+      <c r="G390" s="8">
+        <v>128</v>
+      </c>
+      <c r="H390" s="8">
+        <v>128</v>
+      </c>
+      <c r="I390" s="8">
+        <v>10</v>
+      </c>
+      <c r="J390" s="8">
+        <v>10</v>
+      </c>
+      <c r="K390" s="8">
+        <v>0</v>
+      </c>
+      <c r="L390" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M390" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="391" spans="1:14">
+      <c r="A391" t="s">
+        <v>254</v>
+      </c>
+      <c r="B391">
+        <v>15565216</v>
+      </c>
+      <c r="C391" s="2">
+        <v>60000</v>
+      </c>
+      <c r="D391" s="8">
+        <v>1</v>
+      </c>
+      <c r="E391" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F391" s="8">
+        <v>1</v>
+      </c>
+      <c r="G391" s="8">
+        <v>128</v>
+      </c>
+      <c r="H391" s="8">
+        <v>128</v>
+      </c>
+      <c r="I391" s="8">
+        <v>10</v>
+      </c>
+      <c r="J391" s="8">
+        <v>10</v>
+      </c>
+      <c r="K391" s="8">
+        <v>0</v>
+      </c>
+      <c r="L391" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M391" s="8">
+        <v>10</v>
+      </c>
+      <c r="N391" s="8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="392" spans="1:14">
+      <c r="A392" t="s">
+        <v>254</v>
+      </c>
+      <c r="B392">
+        <v>15565218</v>
+      </c>
+      <c r="C392" s="9">
+        <v>100000000</v>
+      </c>
+      <c r="D392" s="8">
+        <v>1</v>
+      </c>
+      <c r="E392" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F392" s="8">
+        <v>1</v>
+      </c>
+      <c r="G392" s="8">
+        <v>256</v>
+      </c>
+      <c r="H392" s="8">
+        <v>256</v>
+      </c>
+      <c r="I392" s="8">
+        <v>10</v>
+      </c>
+      <c r="J392" s="8">
+        <v>10</v>
+      </c>
+      <c r="K392" s="8">
+        <v>0</v>
+      </c>
+      <c r="L392" s="9">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M392" s="8">
+        <v>1</v>
+      </c>
+      <c r="N392" s="8">
+        <v>1E-3</v>
       </c>
     </row>
   </sheetData>
@@ -15553,17 +15702,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B59324F-8BFA-4D0B-8F1B-AB5C69134BD9}">
   <dimension ref="A1:T234"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B234" sqref="B234"/>
+    <sheetView topLeftCell="A219" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A236" sqref="A236:XFD237"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="27.453125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="25.1796875" style="26" customWidth="1"/>
-    <col min="17" max="18" width="13.26953125" customWidth="1"/>
-    <col min="19" max="19" width="24.7265625" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" style="26" customWidth="1"/>
+    <col min="17" max="18" width="13.28515625" customWidth="1"/>
+    <col min="19" max="19" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16">
@@ -22877,7 +23026,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="190" spans="1:17" ht="18.5">
+    <row r="190" spans="1:17" ht="18.75">
       <c r="B190" s="38"/>
       <c r="C190" s="2">
         <v>100000000</v>
@@ -22921,7 +23070,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="195" spans="1:15" ht="18.5">
+    <row r="195" spans="1:15" ht="18.75">
       <c r="B195" s="38">
         <v>20230417223929</v>
       </c>
@@ -22962,7 +23111,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="196" spans="1:15" ht="18.5">
+    <row r="196" spans="1:15" ht="18.75">
       <c r="B196" s="38">
         <v>20230423215417</v>
       </c>
@@ -23009,7 +23158,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="198" spans="1:15" ht="18.5">
+    <row r="198" spans="1:15" ht="18.75">
       <c r="B198" s="38">
         <v>20230417234354</v>
       </c>
@@ -23053,7 +23202,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="199" spans="1:15" ht="18.5">
+    <row r="199" spans="1:15" ht="18.75">
       <c r="B199" s="38">
         <v>20230417235803</v>
       </c>
@@ -23094,7 +23243,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="200" spans="1:15" ht="18.5">
+    <row r="200" spans="1:15" ht="18.75">
       <c r="B200" s="38">
         <v>20230418001339</v>
       </c>
@@ -23138,7 +23287,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="201" spans="1:15" ht="18.5">
+    <row r="201" spans="1:15" ht="18.75">
       <c r="A201" t="s">
         <v>118</v>
       </c>
@@ -23185,7 +23334,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="202" spans="1:15" ht="18.5">
+    <row r="202" spans="1:15" ht="18.75">
       <c r="B202" s="38"/>
       <c r="C202" s="26">
         <v>10600</v>
@@ -23224,7 +23373,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="203" spans="1:15" ht="18.5">
+    <row r="203" spans="1:15" ht="18.75">
       <c r="A203" s="38">
         <v>20230417232841</v>
       </c>
@@ -23268,7 +23417,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="204" spans="1:15" s="16" customFormat="1" ht="18.5">
+    <row r="204" spans="1:15" s="16" customFormat="1" ht="18.75">
       <c r="A204" s="40" t="s">
         <v>118</v>
       </c>
@@ -23315,7 +23464,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="205" spans="1:15" s="16" customFormat="1" ht="18.5">
+    <row r="205" spans="1:15" s="16" customFormat="1" ht="18.75">
       <c r="A205" s="40" t="s">
         <v>118</v>
       </c>
@@ -23362,7 +23511,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="206" spans="1:15" ht="18.5">
+    <row r="206" spans="1:15" ht="18.75">
       <c r="A206" s="38">
         <v>20230417232841</v>
       </c>
@@ -23406,7 +23555,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="207" spans="1:15" ht="18.5">
+    <row r="207" spans="1:15" ht="18.75">
       <c r="A207" s="38">
         <v>20230417232841</v>
       </c>
@@ -23453,7 +23602,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="208" spans="1:15" ht="18.5">
+    <row r="208" spans="1:15" ht="18.75">
       <c r="A208" s="38">
         <v>20230417232841</v>
       </c>
@@ -23500,7 +23649,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="209" spans="1:15" ht="18.5">
+    <row r="209" spans="1:15" ht="18.75">
       <c r="B209" s="38">
         <v>20230423104141</v>
       </c>
@@ -23544,7 +23693,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="210" spans="1:15" s="16" customFormat="1" ht="18.5">
+    <row r="210" spans="1:15" s="16" customFormat="1" ht="18.75">
       <c r="B210" s="40"/>
       <c r="C210" s="28">
         <v>11000</v>
@@ -23583,7 +23732,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="211" spans="1:15" ht="18.5">
+    <row r="211" spans="1:15" ht="18.75">
       <c r="B211" s="38">
         <v>20230427230257</v>
       </c>
@@ -23627,7 +23776,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="212" spans="1:15" ht="18.5">
+    <row r="212" spans="1:15" ht="18.75">
       <c r="B212" s="38"/>
       <c r="C212" s="26">
         <v>12000</v>
@@ -23666,7 +23815,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="213" spans="1:15" ht="18.5">
+    <row r="213" spans="1:15" ht="18.75">
       <c r="B213" s="38">
         <v>20230427232001</v>
       </c>
@@ -23710,7 +23859,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="214" spans="1:15" ht="18.5">
+    <row r="214" spans="1:15" ht="18.75">
       <c r="B214" s="38">
         <v>20230427224222</v>
       </c>
@@ -24257,7 +24406,7 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
@@ -24982,19 +25131,19 @@
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.453125" style="19" customWidth="1"/>
-    <col min="2" max="2" width="15.1796875" style="19" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="19"/>
-    <col min="5" max="5" width="13.54296875" style="19" customWidth="1"/>
-    <col min="6" max="9" width="8.81640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" style="19"/>
-    <col min="11" max="11" width="18.1796875" style="19" customWidth="1"/>
-    <col min="12" max="12" width="15.453125" style="19" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.7265625" style="19"/>
+    <col min="1" max="1" width="22.42578125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="19"/>
+    <col min="5" max="5" width="13.5703125" style="19" customWidth="1"/>
+    <col min="6" max="9" width="8.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="19"/>
+    <col min="11" max="11" width="18.140625" style="19" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" style="19" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.7109375" style="19"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:14">
@@ -26211,11 +26360,11 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.7265625" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="4" max="4" width="16.54296875" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -26332,22 +26481,24 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C73000ED-ACF1-4870-B376-DD86BAB5368D}">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="26.1796875" style="18" customWidth="1"/>
-    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.81640625" customWidth="1"/>
-    <col min="12" max="12" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.85546875" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -27461,7 +27612,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:17">
       <c r="A33" t="s">
         <v>247</v>
       </c>
@@ -27505,7 +27656,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:17">
       <c r="A34" t="s">
         <v>248</v>
       </c>
@@ -27547,6 +27698,55 @@
       </c>
       <c r="P34" t="s">
         <v>249</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="A36" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="C37" s="31">
+        <v>100</v>
+      </c>
+      <c r="D37" s="31">
+        <v>35</v>
+      </c>
+      <c r="E37" s="31">
+        <v>0</v>
+      </c>
+      <c r="F37" s="31">
+        <v>10</v>
+      </c>
+      <c r="G37" s="31">
+        <v>256</v>
+      </c>
+      <c r="H37" s="31">
+        <v>64</v>
+      </c>
+      <c r="I37" s="31">
+        <v>0</v>
+      </c>
+      <c r="J37" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="L37" s="31">
+        <v>5</v>
+      </c>
+      <c r="M37" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N37" s="31">
+        <v>30</v>
+      </c>
+      <c r="O37" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P37" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -27562,9 +27762,9 @@
       <selection activeCell="A12" sqref="A12:A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.08984375" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">

</xml_diff>

<commit_message>
Update uconn slurm job
</commit_message>
<xml_diff>
--- a/dedalus_case.xlsx
+++ b/dedalus_case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nutstore\Nutstore\Workspace\dedalus_main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2484EBDE-92C1-4454-99FB-DE24BA2AC03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69ECF6E7-56E8-4B42-ACDB-15291C108AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="1950" windowWidth="21600" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RBC flux" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1583" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1698" uniqueCount="278">
   <si>
     <t>slurm_num</t>
   </si>
@@ -826,6 +826,57 @@
   <si>
     <t>beta=0.1</t>
   </si>
+  <si>
+    <t>beta=1000</t>
+  </si>
+  <si>
+    <t>beta=1e4</t>
+  </si>
+  <si>
+    <t>Update 2023/08/27 generate localized structures with different resolutions</t>
+  </si>
+  <si>
+    <t>Expected TKE</t>
+  </si>
+  <si>
+    <t>Lx=10, Nx=128</t>
+  </si>
+  <si>
+    <t>Lx=10, Nx=64</t>
+  </si>
+  <si>
+    <t>Lx=10, Nx=32</t>
+  </si>
+  <si>
+    <t>Lx=10, Nx=16</t>
+  </si>
+  <si>
+    <t>Lx=20, Nx=512</t>
+  </si>
+  <si>
+    <t>Lx=40, Nx=1024</t>
+  </si>
+  <si>
+    <t>34.098047 (still increasing)</t>
+  </si>
+  <si>
+    <t>48.59(still increasing)</t>
+  </si>
+  <si>
+    <t>Lx=10, Nx=256 long run</t>
+  </si>
+  <si>
+    <t>34.788964 (still increasing)</t>
+  </si>
+  <si>
+    <t>50.311298(still increasing)</t>
+  </si>
+  <si>
+    <t>initial_phase=0</t>
+  </si>
+  <si>
+    <t>initial_phase=pi/2</t>
+  </si>
 </sst>
 </file>
 
@@ -940,7 +991,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -996,6 +1047,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1276,22 +1328,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S402"/>
+  <dimension ref="A1:S406"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A392" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B398" sqref="B398"/>
+    <sheetView topLeftCell="A399" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C406" sqref="C406:N406"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" customWidth="1"/>
+    <col min="10" max="10" width="11.7265625" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" customWidth="1"/>
+    <col min="12" max="12" width="14.81640625" customWidth="1"/>
+    <col min="13" max="13" width="14.54296875" customWidth="1"/>
+    <col min="16" max="16" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15">
@@ -2466,7 +2518,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="24" customFormat="1" ht="18.75">
+    <row r="38" spans="1:16" s="24" customFormat="1" ht="18.5">
       <c r="B38" s="51">
         <v>14673046</v>
       </c>
@@ -2541,7 +2593,7 @@
       </c>
       <c r="C43" s="2"/>
     </row>
-    <row r="44" spans="1:16" ht="18.75">
+    <row r="44" spans="1:16" ht="18.5">
       <c r="B44" s="3">
         <v>14541125</v>
       </c>
@@ -2588,7 +2640,7 @@
         <v>12.0533</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="18.75">
+    <row r="45" spans="1:16" ht="18.5">
       <c r="B45" s="3">
         <v>14541126</v>
       </c>
@@ -2635,7 +2687,7 @@
         <v>12.0533</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="18.75">
+    <row r="46" spans="1:16" ht="18.5">
       <c r="B46" s="3">
         <v>14541127</v>
       </c>
@@ -2682,7 +2734,7 @@
         <v>12.0533</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="18.75">
+    <row r="47" spans="1:16" ht="18.5">
       <c r="B47" s="3">
         <v>14541128</v>
       </c>
@@ -2819,7 +2871,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="56" spans="2:16" ht="18.75">
+    <row r="56" spans="2:16" ht="18.5">
       <c r="B56" s="3">
         <v>14673046</v>
       </c>
@@ -2863,7 +2915,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="2:16" ht="18.75">
+    <row r="57" spans="2:16" ht="18.5">
       <c r="B57" s="3">
         <v>14673047</v>
       </c>
@@ -2907,7 +2959,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="2:16" ht="18.75">
+    <row r="58" spans="2:16" ht="18.5">
       <c r="B58" s="3">
         <v>14768718</v>
       </c>
@@ -2948,7 +3000,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="59" spans="2:16" ht="18.75">
+    <row r="59" spans="2:16" ht="18.5">
       <c r="B59" s="3">
         <v>14680791</v>
       </c>
@@ -2992,7 +3044,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="2:16" ht="18.75">
+    <row r="60" spans="2:16" ht="18.5">
       <c r="B60" s="3">
         <v>14741869</v>
       </c>
@@ -3036,7 +3088,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="2:16" ht="18.75">
+    <row r="61" spans="2:16" ht="18.5">
       <c r="B61" s="3">
         <v>14673849</v>
       </c>
@@ -3077,7 +3129,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="62" spans="2:16" ht="18.75">
+    <row r="62" spans="2:16" ht="18.5">
       <c r="B62" s="3">
         <v>14673048</v>
       </c>
@@ -3121,7 +3173,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="2:16" ht="18.75">
+    <row r="63" spans="2:16" ht="18.5">
       <c r="B63" s="3">
         <v>14673049</v>
       </c>
@@ -3255,7 +3307,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="68" spans="2:15" ht="18.75">
+    <row r="68" spans="2:15" ht="18.5">
       <c r="B68" s="3">
         <v>14680810</v>
       </c>
@@ -3299,7 +3351,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="2:15" ht="18.75">
+    <row r="69" spans="2:15" ht="18.5">
       <c r="B69" s="3">
         <v>14672941</v>
       </c>
@@ -3343,7 +3395,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="2:15" ht="18.75">
+    <row r="70" spans="2:15" ht="18.5">
       <c r="B70" s="3">
         <v>14672942</v>
       </c>
@@ -3387,7 +3439,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="2:15" ht="18.75">
+    <row r="71" spans="2:15" ht="18.5">
       <c r="B71" s="3">
         <v>14672943</v>
       </c>
@@ -3431,7 +3483,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="2:15" ht="18.75">
+    <row r="72" spans="2:15" ht="18.5">
       <c r="B72" s="3">
         <v>14672940</v>
       </c>
@@ -3475,7 +3527,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="73" spans="2:15" ht="18">
+    <row r="73" spans="2:15" ht="17.5">
       <c r="B73" s="4">
         <v>14671572</v>
       </c>
@@ -3519,7 +3571,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="74" spans="2:15" ht="18">
+    <row r="74" spans="2:15" ht="17.5">
       <c r="B74" s="4">
         <v>14680814</v>
       </c>
@@ -3563,7 +3615,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="2:15" ht="18">
+    <row r="75" spans="2:15" ht="17.5">
       <c r="B75" s="4">
         <v>14671573</v>
       </c>
@@ -15728,7 +15780,7 @@
         <v>259</v>
       </c>
       <c r="B396">
-        <v>15597574</v>
+        <v>15597575</v>
       </c>
       <c r="C396" s="2">
         <v>60000</v>
@@ -15776,6 +15828,9 @@
       <c r="A398" t="s">
         <v>259</v>
       </c>
+      <c r="B398">
+        <v>15597576</v>
+      </c>
       <c r="C398" s="2">
         <v>60000</v>
       </c>
@@ -15822,6 +15877,9 @@
       <c r="A400" t="s">
         <v>259</v>
       </c>
+      <c r="B400">
+        <v>15597577</v>
+      </c>
       <c r="C400" s="2">
         <v>60000</v>
       </c>
@@ -15868,6 +15926,9 @@
       <c r="A402" t="s">
         <v>259</v>
       </c>
+      <c r="B402">
+        <v>15597578</v>
+      </c>
       <c r="C402" s="2">
         <v>60000</v>
       </c>
@@ -15902,6 +15963,104 @@
         <v>10</v>
       </c>
       <c r="N402" s="8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="403" spans="1:14">
+      <c r="A403" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="404" spans="1:14">
+      <c r="A404" t="s">
+        <v>259</v>
+      </c>
+      <c r="B404">
+        <v>15597579</v>
+      </c>
+      <c r="C404" s="2">
+        <v>60000</v>
+      </c>
+      <c r="D404" s="8">
+        <v>1</v>
+      </c>
+      <c r="E404" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F404" s="8">
+        <v>1</v>
+      </c>
+      <c r="G404" s="8">
+        <v>128</v>
+      </c>
+      <c r="H404" s="8">
+        <v>128</v>
+      </c>
+      <c r="I404" s="8">
+        <v>10</v>
+      </c>
+      <c r="J404" s="8">
+        <v>10</v>
+      </c>
+      <c r="K404" s="8">
+        <v>0</v>
+      </c>
+      <c r="L404" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M404" s="8">
+        <v>10</v>
+      </c>
+      <c r="N404" s="8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="405" spans="1:14">
+      <c r="A405" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="406" spans="1:14">
+      <c r="A406" t="s">
+        <v>259</v>
+      </c>
+      <c r="B406">
+        <v>15565231</v>
+      </c>
+      <c r="C406" s="2">
+        <v>60000</v>
+      </c>
+      <c r="D406" s="8">
+        <v>1</v>
+      </c>
+      <c r="E406" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F406" s="8">
+        <v>1</v>
+      </c>
+      <c r="G406" s="8">
+        <v>128</v>
+      </c>
+      <c r="H406" s="8">
+        <v>128</v>
+      </c>
+      <c r="I406" s="8">
+        <v>10</v>
+      </c>
+      <c r="J406" s="8">
+        <v>10</v>
+      </c>
+      <c r="K406" s="8">
+        <v>0</v>
+      </c>
+      <c r="L406" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="M406" s="8">
+        <v>10</v>
+      </c>
+      <c r="N406" s="8">
         <v>0.01</v>
       </c>
     </row>
@@ -15919,13 +16078,13 @@
       <selection activeCell="A236" sqref="A236:XFD237"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" style="26" customWidth="1"/>
-    <col min="17" max="18" width="13.28515625" customWidth="1"/>
-    <col min="19" max="19" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.453125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="25.1796875" style="26" customWidth="1"/>
+    <col min="17" max="18" width="13.26953125" customWidth="1"/>
+    <col min="19" max="19" width="24.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16">
@@ -23239,7 +23398,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="190" spans="1:17" ht="18.75">
+    <row r="190" spans="1:17" ht="18.5">
       <c r="B190" s="38"/>
       <c r="C190" s="2">
         <v>100000000</v>
@@ -23283,7 +23442,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="195" spans="1:15" ht="18.75">
+    <row r="195" spans="1:15" ht="18.5">
       <c r="B195" s="38">
         <v>20230417223929</v>
       </c>
@@ -23324,7 +23483,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="196" spans="1:15" ht="18.75">
+    <row r="196" spans="1:15" ht="18.5">
       <c r="B196" s="38">
         <v>20230423215417</v>
       </c>
@@ -23371,7 +23530,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="198" spans="1:15" ht="18.75">
+    <row r="198" spans="1:15" ht="18.5">
       <c r="B198" s="38">
         <v>20230417234354</v>
       </c>
@@ -23415,7 +23574,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="199" spans="1:15" ht="18.75">
+    <row r="199" spans="1:15" ht="18.5">
       <c r="B199" s="38">
         <v>20230417235803</v>
       </c>
@@ -23456,7 +23615,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="200" spans="1:15" ht="18.75">
+    <row r="200" spans="1:15" ht="18.5">
       <c r="B200" s="38">
         <v>20230418001339</v>
       </c>
@@ -23500,7 +23659,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="201" spans="1:15" ht="18.75">
+    <row r="201" spans="1:15" ht="18.5">
       <c r="A201" t="s">
         <v>118</v>
       </c>
@@ -23547,7 +23706,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="202" spans="1:15" ht="18.75">
+    <row r="202" spans="1:15" ht="18.5">
       <c r="B202" s="38"/>
       <c r="C202" s="26">
         <v>10600</v>
@@ -23586,7 +23745,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="203" spans="1:15" ht="18.75">
+    <row r="203" spans="1:15" ht="18.5">
       <c r="A203" s="38">
         <v>20230417232841</v>
       </c>
@@ -23630,7 +23789,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="204" spans="1:15" s="16" customFormat="1" ht="18.75">
+    <row r="204" spans="1:15" s="16" customFormat="1" ht="18.5">
       <c r="A204" s="40" t="s">
         <v>118</v>
       </c>
@@ -23677,7 +23836,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="205" spans="1:15" s="16" customFormat="1" ht="18.75">
+    <row r="205" spans="1:15" s="16" customFormat="1" ht="18.5">
       <c r="A205" s="40" t="s">
         <v>118</v>
       </c>
@@ -23724,7 +23883,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="206" spans="1:15" ht="18.75">
+    <row r="206" spans="1:15" ht="18.5">
       <c r="A206" s="38">
         <v>20230417232841</v>
       </c>
@@ -23768,7 +23927,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="207" spans="1:15" ht="18.75">
+    <row r="207" spans="1:15" ht="18.5">
       <c r="A207" s="38">
         <v>20230417232841</v>
       </c>
@@ -23815,7 +23974,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="208" spans="1:15" ht="18.75">
+    <row r="208" spans="1:15" ht="18.5">
       <c r="A208" s="38">
         <v>20230417232841</v>
       </c>
@@ -23862,7 +24021,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="209" spans="1:15" ht="18.75">
+    <row r="209" spans="1:15" ht="18.5">
       <c r="B209" s="38">
         <v>20230423104141</v>
       </c>
@@ -23906,7 +24065,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="210" spans="1:15" s="16" customFormat="1" ht="18.75">
+    <row r="210" spans="1:15" s="16" customFormat="1" ht="18.5">
       <c r="B210" s="40"/>
       <c r="C210" s="28">
         <v>11000</v>
@@ -23945,7 +24104,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="211" spans="1:15" ht="18.75">
+    <row r="211" spans="1:15" ht="18.5">
       <c r="B211" s="38">
         <v>20230427230257</v>
       </c>
@@ -23989,7 +24148,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="212" spans="1:15" ht="18.75">
+    <row r="212" spans="1:15" ht="18.5">
       <c r="B212" s="38"/>
       <c r="C212" s="26">
         <v>12000</v>
@@ -24028,7 +24187,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="213" spans="1:15" ht="18.75">
+    <row r="213" spans="1:15" ht="18.5">
       <c r="B213" s="38">
         <v>20230427232001</v>
       </c>
@@ -24072,7 +24231,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="214" spans="1:15" ht="18.75">
+    <row r="214" spans="1:15" ht="18.5">
       <c r="B214" s="38">
         <v>20230427224222</v>
       </c>
@@ -24619,7 +24778,7 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
@@ -25344,19 +25503,19 @@
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="19" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="19" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="19"/>
-    <col min="5" max="5" width="13.5703125" style="19" customWidth="1"/>
-    <col min="6" max="9" width="8.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" style="19"/>
-    <col min="11" max="11" width="18.140625" style="19" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" style="19" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.7109375" style="19"/>
+    <col min="1" max="1" width="22.453125" style="19" customWidth="1"/>
+    <col min="2" max="2" width="15.1796875" style="19" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="19"/>
+    <col min="5" max="5" width="13.54296875" style="19" customWidth="1"/>
+    <col min="6" max="9" width="8.81640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" style="19"/>
+    <col min="11" max="11" width="18.1796875" style="19" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" style="19" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.7265625" style="19"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:14">
@@ -26573,11 +26732,11 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -26694,24 +26853,25 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C73000ED-ACF1-4870-B376-DD86BAB5368D}">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:R89"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="26.140625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.85546875" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" style="18" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
+    <col min="5" max="5" width="16.26953125" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.81640625" customWidth="1"/>
+    <col min="11" max="11" width="13.7265625" customWidth="1"/>
+    <col min="12" max="12" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -27825,7 +27985,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:18">
       <c r="A33" t="s">
         <v>247</v>
       </c>
@@ -27869,7 +28029,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:18">
       <c r="A34" t="s">
         <v>248</v>
       </c>
@@ -27913,12 +28073,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:18">
       <c r="A36" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:18">
       <c r="C37" s="31">
         <v>100</v>
       </c>
@@ -27960,6 +28120,1739 @@
       </c>
       <c r="Q37" t="s">
         <v>252</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="A40" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>151</v>
+      </c>
+      <c r="R40" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="A41" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" s="16" customFormat="1">
+      <c r="B42" s="27">
+        <v>498554</v>
+      </c>
+      <c r="C42" s="53">
+        <v>100</v>
+      </c>
+      <c r="D42" s="53">
+        <v>35</v>
+      </c>
+      <c r="E42" s="53">
+        <v>0</v>
+      </c>
+      <c r="F42" s="53">
+        <v>10</v>
+      </c>
+      <c r="G42" s="53">
+        <v>256</v>
+      </c>
+      <c r="H42" s="53">
+        <v>64</v>
+      </c>
+      <c r="I42" s="53">
+        <v>0</v>
+      </c>
+      <c r="J42" s="53" t="s">
+        <v>148</v>
+      </c>
+      <c r="K42" s="53">
+        <v>1</v>
+      </c>
+      <c r="L42" s="53">
+        <v>1</v>
+      </c>
+      <c r="M42" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N42" s="53">
+        <v>1000</v>
+      </c>
+      <c r="O42" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="P42" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q42" s="53">
+        <v>18.0412</v>
+      </c>
+      <c r="R42" s="53">
+        <v>18.0412</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" s="16" customFormat="1">
+      <c r="B43" s="27">
+        <v>498545</v>
+      </c>
+      <c r="C43" s="53">
+        <v>100</v>
+      </c>
+      <c r="D43" s="53">
+        <v>35</v>
+      </c>
+      <c r="E43" s="53">
+        <v>0</v>
+      </c>
+      <c r="F43" s="53">
+        <v>10</v>
+      </c>
+      <c r="G43" s="53">
+        <v>256</v>
+      </c>
+      <c r="H43" s="53">
+        <v>64</v>
+      </c>
+      <c r="I43" s="53">
+        <v>0</v>
+      </c>
+      <c r="J43" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K43" s="53"/>
+      <c r="L43" s="53">
+        <v>5</v>
+      </c>
+      <c r="M43" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N43" s="53">
+        <v>1000</v>
+      </c>
+      <c r="O43" s="53">
+        <v>10</v>
+      </c>
+      <c r="P43" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q43" s="53" t="s">
+        <v>274</v>
+      </c>
+      <c r="R43" s="16" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" s="16" customFormat="1">
+      <c r="B44" s="27">
+        <v>498551</v>
+      </c>
+      <c r="C44" s="53">
+        <v>100</v>
+      </c>
+      <c r="D44" s="53">
+        <v>35</v>
+      </c>
+      <c r="E44" s="53">
+        <v>0</v>
+      </c>
+      <c r="F44" s="53">
+        <v>10</v>
+      </c>
+      <c r="G44" s="53">
+        <v>256</v>
+      </c>
+      <c r="H44" s="53">
+        <v>64</v>
+      </c>
+      <c r="I44" s="53">
+        <v>0</v>
+      </c>
+      <c r="J44" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K44" s="53"/>
+      <c r="L44" s="53">
+        <v>2</v>
+      </c>
+      <c r="M44" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N44" s="53">
+        <v>1000</v>
+      </c>
+      <c r="O44" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="P44" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q44" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="R44" s="16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" s="16" customFormat="1">
+      <c r="B45" s="27">
+        <v>498552</v>
+      </c>
+      <c r="C45" s="53">
+        <v>100</v>
+      </c>
+      <c r="D45" s="53">
+        <v>35</v>
+      </c>
+      <c r="E45" s="53">
+        <v>0</v>
+      </c>
+      <c r="F45" s="53">
+        <v>10</v>
+      </c>
+      <c r="G45" s="53">
+        <v>256</v>
+      </c>
+      <c r="H45" s="53">
+        <v>64</v>
+      </c>
+      <c r="I45" s="53">
+        <v>0</v>
+      </c>
+      <c r="J45" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K45" s="53"/>
+      <c r="L45" s="53">
+        <v>4</v>
+      </c>
+      <c r="M45" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N45" s="53">
+        <v>1000</v>
+      </c>
+      <c r="O45" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="P45" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q45" s="16">
+        <v>56.929834999999997</v>
+      </c>
+      <c r="R45" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" s="16" customFormat="1">
+      <c r="B46" s="27">
+        <v>498553</v>
+      </c>
+      <c r="C46" s="53">
+        <v>100</v>
+      </c>
+      <c r="D46" s="53">
+        <v>35</v>
+      </c>
+      <c r="E46" s="53">
+        <v>0</v>
+      </c>
+      <c r="F46" s="53">
+        <v>10</v>
+      </c>
+      <c r="G46" s="53">
+        <v>256</v>
+      </c>
+      <c r="H46" s="53">
+        <v>64</v>
+      </c>
+      <c r="I46" s="53">
+        <v>0</v>
+      </c>
+      <c r="J46" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K46" s="53" t="s">
+        <v>277</v>
+      </c>
+      <c r="L46" s="53">
+        <v>3</v>
+      </c>
+      <c r="M46" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N46" s="53">
+        <v>1000</v>
+      </c>
+      <c r="O46" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="P46" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="R46" s="53">
+        <v>57.424432000000003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" s="16" customFormat="1">
+      <c r="B47" s="27">
+        <v>504615</v>
+      </c>
+      <c r="C47" s="53">
+        <v>100</v>
+      </c>
+      <c r="D47" s="53">
+        <v>35</v>
+      </c>
+      <c r="E47" s="53">
+        <v>0</v>
+      </c>
+      <c r="F47" s="53">
+        <v>10</v>
+      </c>
+      <c r="G47" s="53">
+        <v>256</v>
+      </c>
+      <c r="H47" s="53">
+        <v>64</v>
+      </c>
+      <c r="I47" s="53">
+        <v>0</v>
+      </c>
+      <c r="J47" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K47" s="53" t="s">
+        <v>276</v>
+      </c>
+      <c r="L47" s="53">
+        <v>3</v>
+      </c>
+      <c r="M47" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N47" s="53">
+        <v>1000</v>
+      </c>
+      <c r="O47" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="P47" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="R47" s="53">
+        <v>57.424432000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" s="16" customFormat="1">
+      <c r="A49" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="B49" s="27"/>
+    </row>
+    <row r="50" spans="1:18">
+      <c r="B50" s="18">
+        <v>498184</v>
+      </c>
+      <c r="C50" s="31">
+        <v>100</v>
+      </c>
+      <c r="D50" s="31">
+        <v>35</v>
+      </c>
+      <c r="E50" s="31">
+        <v>0</v>
+      </c>
+      <c r="F50" s="31">
+        <v>10</v>
+      </c>
+      <c r="G50" s="31">
+        <v>128</v>
+      </c>
+      <c r="H50" s="31">
+        <v>64</v>
+      </c>
+      <c r="I50" s="31">
+        <v>0</v>
+      </c>
+      <c r="J50" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="K50" s="31">
+        <v>1</v>
+      </c>
+      <c r="L50" s="31">
+        <v>1</v>
+      </c>
+      <c r="M50" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N50" s="31">
+        <v>10</v>
+      </c>
+      <c r="O50" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P50" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q50" s="31">
+        <v>18.041212000000002</v>
+      </c>
+      <c r="R50" s="31">
+        <v>18.0412</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18">
+      <c r="B51" s="18">
+        <v>498190</v>
+      </c>
+      <c r="C51" s="31">
+        <v>100</v>
+      </c>
+      <c r="D51" s="31">
+        <v>35</v>
+      </c>
+      <c r="E51" s="31">
+        <v>0</v>
+      </c>
+      <c r="F51" s="31">
+        <v>10</v>
+      </c>
+      <c r="G51" s="31">
+        <v>128</v>
+      </c>
+      <c r="H51" s="31">
+        <v>64</v>
+      </c>
+      <c r="I51" s="31">
+        <v>0</v>
+      </c>
+      <c r="J51" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K51" s="31"/>
+      <c r="L51" s="31">
+        <v>5</v>
+      </c>
+      <c r="M51" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N51" s="31">
+        <v>10</v>
+      </c>
+      <c r="O51" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P51" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q51" s="31" t="s">
+        <v>271</v>
+      </c>
+      <c r="R51" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18">
+      <c r="B52" s="18">
+        <v>498197</v>
+      </c>
+      <c r="C52" s="31">
+        <v>100</v>
+      </c>
+      <c r="D52" s="31">
+        <v>35</v>
+      </c>
+      <c r="E52" s="31">
+        <v>0</v>
+      </c>
+      <c r="F52" s="31">
+        <v>10</v>
+      </c>
+      <c r="G52" s="31">
+        <v>128</v>
+      </c>
+      <c r="H52" s="31">
+        <v>64</v>
+      </c>
+      <c r="I52" s="31">
+        <v>0</v>
+      </c>
+      <c r="J52" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K52" s="31"/>
+      <c r="L52" s="53">
+        <v>2</v>
+      </c>
+      <c r="M52" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N52" s="31">
+        <v>10</v>
+      </c>
+      <c r="O52" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P52" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>272</v>
+      </c>
+      <c r="R52" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18">
+      <c r="C53" s="31">
+        <v>100</v>
+      </c>
+      <c r="D53" s="31">
+        <v>35</v>
+      </c>
+      <c r="E53" s="31">
+        <v>0</v>
+      </c>
+      <c r="F53" s="31">
+        <v>10</v>
+      </c>
+      <c r="G53" s="31">
+        <v>128</v>
+      </c>
+      <c r="H53" s="31">
+        <v>64</v>
+      </c>
+      <c r="I53" s="31">
+        <v>0</v>
+      </c>
+      <c r="J53" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K53" s="31"/>
+      <c r="L53" s="31">
+        <v>4</v>
+      </c>
+      <c r="M53" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N53" s="31">
+        <v>10</v>
+      </c>
+      <c r="O53" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P53" t="s">
+        <v>144</v>
+      </c>
+      <c r="R53" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18">
+      <c r="C54" s="31">
+        <v>100</v>
+      </c>
+      <c r="D54" s="31">
+        <v>35</v>
+      </c>
+      <c r="E54" s="31">
+        <v>0</v>
+      </c>
+      <c r="F54" s="31">
+        <v>10</v>
+      </c>
+      <c r="G54" s="31">
+        <v>128</v>
+      </c>
+      <c r="H54" s="31">
+        <v>64</v>
+      </c>
+      <c r="I54" s="31">
+        <v>0</v>
+      </c>
+      <c r="J54" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K54" s="31"/>
+      <c r="L54" s="31">
+        <v>3</v>
+      </c>
+      <c r="M54" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N54" s="31">
+        <v>10</v>
+      </c>
+      <c r="O54" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P54" t="s">
+        <v>143</v>
+      </c>
+      <c r="R54" s="31">
+        <v>57.424432000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18">
+      <c r="A56" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18">
+      <c r="C57" s="31">
+        <v>100</v>
+      </c>
+      <c r="D57" s="31">
+        <v>35</v>
+      </c>
+      <c r="E57" s="31">
+        <v>0</v>
+      </c>
+      <c r="F57" s="31">
+        <v>10</v>
+      </c>
+      <c r="G57" s="31">
+        <v>64</v>
+      </c>
+      <c r="H57" s="31">
+        <v>64</v>
+      </c>
+      <c r="I57" s="31">
+        <v>0</v>
+      </c>
+      <c r="J57" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="K57" s="31">
+        <v>1</v>
+      </c>
+      <c r="L57" s="31">
+        <v>1</v>
+      </c>
+      <c r="M57" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N57" s="31">
+        <v>10</v>
+      </c>
+      <c r="O57" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P57" t="s">
+        <v>149</v>
+      </c>
+      <c r="R57" s="31">
+        <v>18.0412</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18">
+      <c r="C58" s="31">
+        <v>100</v>
+      </c>
+      <c r="D58" s="31">
+        <v>35</v>
+      </c>
+      <c r="E58" s="31">
+        <v>0</v>
+      </c>
+      <c r="F58" s="31">
+        <v>10</v>
+      </c>
+      <c r="G58" s="31">
+        <v>64</v>
+      </c>
+      <c r="H58" s="31">
+        <v>64</v>
+      </c>
+      <c r="I58" s="31">
+        <v>0</v>
+      </c>
+      <c r="J58" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K58" s="31"/>
+      <c r="L58" s="31">
+        <v>5</v>
+      </c>
+      <c r="M58" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N58" s="31">
+        <v>10</v>
+      </c>
+      <c r="O58" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P58" t="s">
+        <v>142</v>
+      </c>
+      <c r="R58" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18">
+      <c r="C59" s="31">
+        <v>100</v>
+      </c>
+      <c r="D59" s="31">
+        <v>35</v>
+      </c>
+      <c r="E59" s="31">
+        <v>0</v>
+      </c>
+      <c r="F59" s="31">
+        <v>10</v>
+      </c>
+      <c r="G59" s="31">
+        <v>64</v>
+      </c>
+      <c r="H59" s="31">
+        <v>64</v>
+      </c>
+      <c r="I59" s="31">
+        <v>0</v>
+      </c>
+      <c r="J59" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K59" s="31"/>
+      <c r="L59" s="31">
+        <v>1</v>
+      </c>
+      <c r="M59" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N59" s="31">
+        <v>10</v>
+      </c>
+      <c r="O59" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P59" t="s">
+        <v>141</v>
+      </c>
+      <c r="R59" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18">
+      <c r="C60" s="31">
+        <v>100</v>
+      </c>
+      <c r="D60" s="31">
+        <v>35</v>
+      </c>
+      <c r="E60" s="31">
+        <v>0</v>
+      </c>
+      <c r="F60" s="31">
+        <v>10</v>
+      </c>
+      <c r="G60" s="31">
+        <v>64</v>
+      </c>
+      <c r="H60" s="31">
+        <v>64</v>
+      </c>
+      <c r="I60" s="31">
+        <v>0</v>
+      </c>
+      <c r="J60" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K60" s="31"/>
+      <c r="L60" s="31">
+        <v>4</v>
+      </c>
+      <c r="M60" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N60" s="31">
+        <v>10</v>
+      </c>
+      <c r="O60" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P60" t="s">
+        <v>144</v>
+      </c>
+      <c r="R60" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18">
+      <c r="C61" s="31">
+        <v>100</v>
+      </c>
+      <c r="D61" s="31">
+        <v>35</v>
+      </c>
+      <c r="E61" s="31">
+        <v>0</v>
+      </c>
+      <c r="F61" s="31">
+        <v>10</v>
+      </c>
+      <c r="G61" s="31">
+        <v>64</v>
+      </c>
+      <c r="H61" s="31">
+        <v>64</v>
+      </c>
+      <c r="I61" s="31">
+        <v>0</v>
+      </c>
+      <c r="J61" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K61" s="31"/>
+      <c r="L61" s="31">
+        <v>3</v>
+      </c>
+      <c r="M61" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N61" s="31">
+        <v>10</v>
+      </c>
+      <c r="O61" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P61" t="s">
+        <v>143</v>
+      </c>
+      <c r="R61" s="31">
+        <v>57.424432000000003</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18">
+      <c r="A63" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18">
+      <c r="C64" s="31">
+        <v>100</v>
+      </c>
+      <c r="D64" s="31">
+        <v>35</v>
+      </c>
+      <c r="E64" s="31">
+        <v>0</v>
+      </c>
+      <c r="F64" s="31">
+        <v>10</v>
+      </c>
+      <c r="G64" s="31">
+        <v>32</v>
+      </c>
+      <c r="H64" s="31">
+        <v>64</v>
+      </c>
+      <c r="I64" s="31">
+        <v>0</v>
+      </c>
+      <c r="J64" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="K64" s="31">
+        <v>1</v>
+      </c>
+      <c r="L64" s="31">
+        <v>1</v>
+      </c>
+      <c r="M64" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N64" s="31">
+        <v>10</v>
+      </c>
+      <c r="O64" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P64" t="s">
+        <v>149</v>
+      </c>
+      <c r="R64" s="31">
+        <v>18.0412</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18">
+      <c r="C65" s="31">
+        <v>100</v>
+      </c>
+      <c r="D65" s="31">
+        <v>35</v>
+      </c>
+      <c r="E65" s="31">
+        <v>0</v>
+      </c>
+      <c r="F65" s="31">
+        <v>10</v>
+      </c>
+      <c r="G65" s="31">
+        <v>32</v>
+      </c>
+      <c r="H65" s="31">
+        <v>64</v>
+      </c>
+      <c r="I65" s="31">
+        <v>0</v>
+      </c>
+      <c r="J65" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K65" s="31"/>
+      <c r="L65" s="31">
+        <v>5</v>
+      </c>
+      <c r="M65" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N65" s="31">
+        <v>10</v>
+      </c>
+      <c r="O65" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P65" t="s">
+        <v>142</v>
+      </c>
+      <c r="R65" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18">
+      <c r="C66" s="31">
+        <v>100</v>
+      </c>
+      <c r="D66" s="31">
+        <v>35</v>
+      </c>
+      <c r="E66" s="31">
+        <v>0</v>
+      </c>
+      <c r="F66" s="31">
+        <v>10</v>
+      </c>
+      <c r="G66" s="31">
+        <v>32</v>
+      </c>
+      <c r="H66" s="31">
+        <v>64</v>
+      </c>
+      <c r="I66" s="31">
+        <v>0</v>
+      </c>
+      <c r="J66" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K66" s="31"/>
+      <c r="L66" s="31">
+        <v>1</v>
+      </c>
+      <c r="M66" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N66" s="31">
+        <v>10</v>
+      </c>
+      <c r="O66" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P66" t="s">
+        <v>141</v>
+      </c>
+      <c r="R66" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18">
+      <c r="C67" s="31">
+        <v>100</v>
+      </c>
+      <c r="D67" s="31">
+        <v>35</v>
+      </c>
+      <c r="E67" s="31">
+        <v>0</v>
+      </c>
+      <c r="F67" s="31">
+        <v>10</v>
+      </c>
+      <c r="G67" s="31">
+        <v>32</v>
+      </c>
+      <c r="H67" s="31">
+        <v>64</v>
+      </c>
+      <c r="I67" s="31">
+        <v>0</v>
+      </c>
+      <c r="J67" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K67" s="31"/>
+      <c r="L67" s="31">
+        <v>4</v>
+      </c>
+      <c r="M67" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N67" s="31">
+        <v>10</v>
+      </c>
+      <c r="O67" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P67" t="s">
+        <v>144</v>
+      </c>
+      <c r="R67" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18">
+      <c r="C68" s="31">
+        <v>100</v>
+      </c>
+      <c r="D68" s="31">
+        <v>35</v>
+      </c>
+      <c r="E68" s="31">
+        <v>0</v>
+      </c>
+      <c r="F68" s="31">
+        <v>10</v>
+      </c>
+      <c r="G68" s="31">
+        <v>32</v>
+      </c>
+      <c r="H68" s="31">
+        <v>64</v>
+      </c>
+      <c r="I68" s="31">
+        <v>0</v>
+      </c>
+      <c r="J68" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K68" s="31"/>
+      <c r="L68" s="31">
+        <v>3</v>
+      </c>
+      <c r="M68" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N68" s="31">
+        <v>10</v>
+      </c>
+      <c r="O68" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P68" t="s">
+        <v>143</v>
+      </c>
+      <c r="R68" s="31">
+        <v>57.424432000000003</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18">
+      <c r="A70" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18">
+      <c r="C71" s="31">
+        <v>100</v>
+      </c>
+      <c r="D71" s="31">
+        <v>35</v>
+      </c>
+      <c r="E71" s="31">
+        <v>0</v>
+      </c>
+      <c r="F71" s="31">
+        <v>10</v>
+      </c>
+      <c r="G71" s="31">
+        <v>16</v>
+      </c>
+      <c r="H71" s="31">
+        <v>64</v>
+      </c>
+      <c r="I71" s="31">
+        <v>0</v>
+      </c>
+      <c r="J71" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="K71" s="31">
+        <v>1</v>
+      </c>
+      <c r="L71" s="31">
+        <v>1</v>
+      </c>
+      <c r="M71" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N71" s="31">
+        <v>10</v>
+      </c>
+      <c r="O71" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P71" t="s">
+        <v>149</v>
+      </c>
+      <c r="R71" s="31">
+        <v>18.0412</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18">
+      <c r="C72" s="31">
+        <v>100</v>
+      </c>
+      <c r="D72" s="31">
+        <v>35</v>
+      </c>
+      <c r="E72" s="31">
+        <v>0</v>
+      </c>
+      <c r="F72" s="31">
+        <v>10</v>
+      </c>
+      <c r="G72" s="31">
+        <v>16</v>
+      </c>
+      <c r="H72" s="31">
+        <v>64</v>
+      </c>
+      <c r="I72" s="31">
+        <v>0</v>
+      </c>
+      <c r="J72" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K72" s="31"/>
+      <c r="L72" s="31">
+        <v>5</v>
+      </c>
+      <c r="M72" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N72" s="31">
+        <v>10</v>
+      </c>
+      <c r="O72" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P72" t="s">
+        <v>142</v>
+      </c>
+      <c r="R72" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18">
+      <c r="C73" s="31">
+        <v>100</v>
+      </c>
+      <c r="D73" s="31">
+        <v>35</v>
+      </c>
+      <c r="E73" s="31">
+        <v>0</v>
+      </c>
+      <c r="F73" s="31">
+        <v>10</v>
+      </c>
+      <c r="G73" s="31">
+        <v>16</v>
+      </c>
+      <c r="H73" s="31">
+        <v>64</v>
+      </c>
+      <c r="I73" s="31">
+        <v>0</v>
+      </c>
+      <c r="J73" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K73" s="31"/>
+      <c r="L73" s="31">
+        <v>1</v>
+      </c>
+      <c r="M73" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N73" s="31">
+        <v>10</v>
+      </c>
+      <c r="O73" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P73" t="s">
+        <v>141</v>
+      </c>
+      <c r="R73" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18">
+      <c r="C74" s="31">
+        <v>100</v>
+      </c>
+      <c r="D74" s="31">
+        <v>35</v>
+      </c>
+      <c r="E74" s="31">
+        <v>0</v>
+      </c>
+      <c r="F74" s="31">
+        <v>10</v>
+      </c>
+      <c r="G74" s="31">
+        <v>16</v>
+      </c>
+      <c r="H74" s="31">
+        <v>64</v>
+      </c>
+      <c r="I74" s="31">
+        <v>0</v>
+      </c>
+      <c r="J74" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K74" s="31"/>
+      <c r="L74" s="31">
+        <v>4</v>
+      </c>
+      <c r="M74" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N74" s="31">
+        <v>10</v>
+      </c>
+      <c r="O74" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P74" t="s">
+        <v>144</v>
+      </c>
+      <c r="R74" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18">
+      <c r="C75" s="31">
+        <v>100</v>
+      </c>
+      <c r="D75" s="31">
+        <v>35</v>
+      </c>
+      <c r="E75" s="31">
+        <v>0</v>
+      </c>
+      <c r="F75" s="31">
+        <v>10</v>
+      </c>
+      <c r="G75" s="31">
+        <v>16</v>
+      </c>
+      <c r="H75" s="31">
+        <v>64</v>
+      </c>
+      <c r="I75" s="31">
+        <v>0</v>
+      </c>
+      <c r="J75" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K75" s="31"/>
+      <c r="L75" s="31">
+        <v>3</v>
+      </c>
+      <c r="M75" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N75" s="31">
+        <v>10</v>
+      </c>
+      <c r="O75" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P75" t="s">
+        <v>143</v>
+      </c>
+      <c r="R75" s="31">
+        <v>57.424432000000003</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18">
+      <c r="A77" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18">
+      <c r="C78" s="31">
+        <v>100</v>
+      </c>
+      <c r="D78" s="31">
+        <v>35</v>
+      </c>
+      <c r="E78" s="31">
+        <v>0</v>
+      </c>
+      <c r="F78" s="31">
+        <v>20</v>
+      </c>
+      <c r="G78" s="31">
+        <v>512</v>
+      </c>
+      <c r="H78" s="31">
+        <v>64</v>
+      </c>
+      <c r="I78" s="31">
+        <v>0</v>
+      </c>
+      <c r="J78" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="K78" s="31">
+        <v>1</v>
+      </c>
+      <c r="L78" s="31">
+        <v>1</v>
+      </c>
+      <c r="M78" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N78" s="31">
+        <v>10</v>
+      </c>
+      <c r="O78" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P78" t="s">
+        <v>149</v>
+      </c>
+      <c r="R78" s="31">
+        <v>18.0412</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18">
+      <c r="C79" s="31">
+        <v>100</v>
+      </c>
+      <c r="D79" s="31">
+        <v>35</v>
+      </c>
+      <c r="E79" s="31">
+        <v>0</v>
+      </c>
+      <c r="F79" s="31">
+        <v>20</v>
+      </c>
+      <c r="G79" s="31">
+        <v>512</v>
+      </c>
+      <c r="H79" s="31">
+        <v>64</v>
+      </c>
+      <c r="I79" s="31">
+        <v>0</v>
+      </c>
+      <c r="J79" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K79" s="31"/>
+      <c r="L79" s="31">
+        <v>5</v>
+      </c>
+      <c r="M79" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N79" s="31">
+        <v>10</v>
+      </c>
+      <c r="O79" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P79" t="s">
+        <v>142</v>
+      </c>
+      <c r="R79" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18">
+      <c r="C80" s="31">
+        <v>100</v>
+      </c>
+      <c r="D80" s="31">
+        <v>35</v>
+      </c>
+      <c r="E80" s="31">
+        <v>0</v>
+      </c>
+      <c r="F80" s="31">
+        <v>20</v>
+      </c>
+      <c r="G80" s="31">
+        <v>512</v>
+      </c>
+      <c r="H80" s="31">
+        <v>64</v>
+      </c>
+      <c r="I80" s="31">
+        <v>0</v>
+      </c>
+      <c r="J80" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K80" s="31"/>
+      <c r="L80" s="31">
+        <v>1</v>
+      </c>
+      <c r="M80" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N80" s="31">
+        <v>10</v>
+      </c>
+      <c r="O80" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P80" t="s">
+        <v>141</v>
+      </c>
+      <c r="R80" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18">
+      <c r="C81" s="31">
+        <v>100</v>
+      </c>
+      <c r="D81" s="31">
+        <v>35</v>
+      </c>
+      <c r="E81" s="31">
+        <v>0</v>
+      </c>
+      <c r="F81" s="31">
+        <v>20</v>
+      </c>
+      <c r="G81" s="31">
+        <v>512</v>
+      </c>
+      <c r="H81" s="31">
+        <v>64</v>
+      </c>
+      <c r="I81" s="31">
+        <v>0</v>
+      </c>
+      <c r="J81" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K81" s="31"/>
+      <c r="L81" s="31">
+        <v>4</v>
+      </c>
+      <c r="M81" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N81" s="31">
+        <v>10</v>
+      </c>
+      <c r="O81" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P81" t="s">
+        <v>144</v>
+      </c>
+      <c r="R81" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18">
+      <c r="C82" s="31">
+        <v>100</v>
+      </c>
+      <c r="D82" s="31">
+        <v>35</v>
+      </c>
+      <c r="E82" s="31">
+        <v>0</v>
+      </c>
+      <c r="F82" s="31">
+        <v>20</v>
+      </c>
+      <c r="G82" s="31">
+        <v>512</v>
+      </c>
+      <c r="H82" s="31">
+        <v>64</v>
+      </c>
+      <c r="I82" s="31">
+        <v>0</v>
+      </c>
+      <c r="J82" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K82" s="31"/>
+      <c r="L82" s="31">
+        <v>3</v>
+      </c>
+      <c r="M82" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N82" s="31">
+        <v>10</v>
+      </c>
+      <c r="O82" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P82" t="s">
+        <v>143</v>
+      </c>
+      <c r="R82" s="31">
+        <v>57.424432000000003</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18">
+      <c r="A84" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18">
+      <c r="C85" s="31">
+        <v>100</v>
+      </c>
+      <c r="D85" s="31">
+        <v>35</v>
+      </c>
+      <c r="E85" s="31">
+        <v>0</v>
+      </c>
+      <c r="F85" s="31">
+        <v>40</v>
+      </c>
+      <c r="G85" s="31">
+        <v>1024</v>
+      </c>
+      <c r="H85" s="31">
+        <v>64</v>
+      </c>
+      <c r="I85" s="31">
+        <v>0</v>
+      </c>
+      <c r="J85" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="K85" s="31">
+        <v>1</v>
+      </c>
+      <c r="L85" s="31">
+        <v>1</v>
+      </c>
+      <c r="M85" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N85" s="31">
+        <v>10</v>
+      </c>
+      <c r="O85" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P85" t="s">
+        <v>149</v>
+      </c>
+      <c r="R85" s="31">
+        <v>18.0412</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18">
+      <c r="C86" s="31">
+        <v>100</v>
+      </c>
+      <c r="D86" s="31">
+        <v>35</v>
+      </c>
+      <c r="E86" s="31">
+        <v>0</v>
+      </c>
+      <c r="F86" s="31">
+        <v>40</v>
+      </c>
+      <c r="G86" s="31">
+        <v>1024</v>
+      </c>
+      <c r="H86" s="31">
+        <v>64</v>
+      </c>
+      <c r="I86" s="31">
+        <v>0</v>
+      </c>
+      <c r="J86" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K86" s="31"/>
+      <c r="L86" s="31">
+        <v>5</v>
+      </c>
+      <c r="M86" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N86" s="31">
+        <v>10</v>
+      </c>
+      <c r="O86" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P86" t="s">
+        <v>142</v>
+      </c>
+      <c r="R86" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18">
+      <c r="C87" s="31">
+        <v>100</v>
+      </c>
+      <c r="D87" s="31">
+        <v>35</v>
+      </c>
+      <c r="E87" s="31">
+        <v>0</v>
+      </c>
+      <c r="F87" s="31">
+        <v>40</v>
+      </c>
+      <c r="G87" s="31">
+        <v>1024</v>
+      </c>
+      <c r="H87" s="31">
+        <v>64</v>
+      </c>
+      <c r="I87" s="31">
+        <v>0</v>
+      </c>
+      <c r="J87" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K87" s="31"/>
+      <c r="L87" s="31">
+        <v>1</v>
+      </c>
+      <c r="M87" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N87" s="31">
+        <v>10</v>
+      </c>
+      <c r="O87" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P87" t="s">
+        <v>141</v>
+      </c>
+      <c r="R87" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18">
+      <c r="C88" s="31">
+        <v>100</v>
+      </c>
+      <c r="D88" s="31">
+        <v>35</v>
+      </c>
+      <c r="E88" s="31">
+        <v>0</v>
+      </c>
+      <c r="F88" s="31">
+        <v>40</v>
+      </c>
+      <c r="G88" s="31">
+        <v>1024</v>
+      </c>
+      <c r="H88" s="31">
+        <v>64</v>
+      </c>
+      <c r="I88" s="31">
+        <v>0</v>
+      </c>
+      <c r="J88" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K88" s="31"/>
+      <c r="L88" s="31">
+        <v>4</v>
+      </c>
+      <c r="M88" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N88" s="31">
+        <v>10</v>
+      </c>
+      <c r="O88" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P88" t="s">
+        <v>144</v>
+      </c>
+      <c r="R88" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18">
+      <c r="C89" s="31">
+        <v>100</v>
+      </c>
+      <c r="D89" s="31">
+        <v>35</v>
+      </c>
+      <c r="E89" s="31">
+        <v>0</v>
+      </c>
+      <c r="F89" s="31">
+        <v>40</v>
+      </c>
+      <c r="G89" s="31">
+        <v>1024</v>
+      </c>
+      <c r="H89" s="31">
+        <v>64</v>
+      </c>
+      <c r="I89" s="31">
+        <v>0</v>
+      </c>
+      <c r="J89" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K89" s="31"/>
+      <c r="L89" s="31">
+        <v>3</v>
+      </c>
+      <c r="M89" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N89" s="31">
+        <v>10</v>
+      </c>
+      <c r="O89" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P89" t="s">
+        <v>143</v>
+      </c>
+      <c r="R89" s="31">
+        <v>57.424432000000003</v>
       </c>
     </row>
   </sheetData>
@@ -27975,9 +29868,9 @@
       <selection activeCell="A12" sqref="A12:A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">

</xml_diff>

<commit_message>
Update the rotation in the formulation
</commit_message>
<xml_diff>
--- a/dedalus_case.xlsx
+++ b/dedalus_case.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nutstore\Nutstore\Workspace\dedalus_main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69ECF6E7-56E8-4B42-ACDB-15291C108AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04F5A2D-FE10-43EE-BAC8-0CE820F4AF1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1698" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1738" uniqueCount="284">
   <si>
     <t>slurm_num</t>
   </si>
@@ -875,7 +875,25 @@
     <t>initial_phase=0</t>
   </si>
   <si>
-    <t>initial_phase=pi/2</t>
+    <t>Lx=15, Nx=384</t>
+  </si>
+  <si>
+    <t>Lx=30, Nx=768</t>
+  </si>
+  <si>
+    <t>0 trivial state</t>
+  </si>
+  <si>
+    <t>18…</t>
+  </si>
+  <si>
+    <t>35….</t>
+  </si>
+  <si>
+    <t>54…</t>
+  </si>
+  <si>
+    <t>58…</t>
   </si>
 </sst>
 </file>
@@ -26853,10 +26871,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C73000ED-ACF1-4870-B376-DD86BAB5368D}">
-  <dimension ref="A1:R89"/>
+  <dimension ref="A1:R108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -28346,7 +28364,7 @@
     </row>
     <row r="46" spans="1:18" s="16" customFormat="1">
       <c r="B46" s="27">
-        <v>498553</v>
+        <v>504615</v>
       </c>
       <c r="C46" s="53">
         <v>100</v>
@@ -28373,7 +28391,7 @@
         <v>146</v>
       </c>
       <c r="K46" s="53" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L46" s="53">
         <v>3</v>
@@ -28396,7 +28414,7 @@
     </row>
     <row r="47" spans="1:18" s="16" customFormat="1">
       <c r="B47" s="27">
-        <v>504615</v>
+        <v>1406676</v>
       </c>
       <c r="C47" s="53">
         <v>100</v>
@@ -28426,7 +28444,7 @@
         <v>276</v>
       </c>
       <c r="L47" s="53">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M47" s="53">
         <v>1E-3</v>
@@ -28438,11 +28456,9 @@
         <v>0.1</v>
       </c>
       <c r="P47" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="R47" s="53">
-        <v>57.424432000000003</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="R47" s="53"/>
     </row>
     <row r="49" spans="1:18" s="16" customFormat="1">
       <c r="A49" s="16" t="s">
@@ -28695,56 +28711,25 @@
         <v>57.424432000000003</v>
       </c>
     </row>
-    <row r="56" spans="1:18">
-      <c r="A56" t="s">
+    <row r="55" spans="1:18">
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="31"/>
+      <c r="H55" s="31"/>
+      <c r="I55" s="31"/>
+      <c r="J55" s="31"/>
+      <c r="K55" s="31"/>
+      <c r="L55" s="31"/>
+      <c r="M55" s="31"/>
+      <c r="N55" s="31"/>
+      <c r="O55" s="31"/>
+      <c r="R55" s="31"/>
+    </row>
+    <row r="57" spans="1:18">
+      <c r="A57" t="s">
         <v>266</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18">
-      <c r="C57" s="31">
-        <v>100</v>
-      </c>
-      <c r="D57" s="31">
-        <v>35</v>
-      </c>
-      <c r="E57" s="31">
-        <v>0</v>
-      </c>
-      <c r="F57" s="31">
-        <v>10</v>
-      </c>
-      <c r="G57" s="31">
-        <v>64</v>
-      </c>
-      <c r="H57" s="31">
-        <v>64</v>
-      </c>
-      <c r="I57" s="31">
-        <v>0</v>
-      </c>
-      <c r="J57" s="31" t="s">
-        <v>148</v>
-      </c>
-      <c r="K57" s="31">
-        <v>1</v>
-      </c>
-      <c r="L57" s="31">
-        <v>1</v>
-      </c>
-      <c r="M57" s="31">
-        <v>1E-3</v>
-      </c>
-      <c r="N57" s="31">
-        <v>10</v>
-      </c>
-      <c r="O57" s="31">
-        <v>0.1</v>
-      </c>
-      <c r="P57" t="s">
-        <v>149</v>
-      </c>
-      <c r="R57" s="31">
-        <v>18.0412</v>
       </c>
     </row>
     <row r="58" spans="1:18">
@@ -28770,11 +28755,13 @@
         <v>0</v>
       </c>
       <c r="J58" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="K58" s="31"/>
+        <v>148</v>
+      </c>
+      <c r="K58" s="31">
+        <v>1</v>
+      </c>
       <c r="L58" s="31">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M58" s="31">
         <v>1E-3</v>
@@ -28786,10 +28773,10 @@
         <v>0.1</v>
       </c>
       <c r="P58" t="s">
-        <v>142</v>
-      </c>
-      <c r="R58" t="s">
-        <v>152</v>
+        <v>149</v>
+      </c>
+      <c r="R58" s="31">
+        <v>18.0412</v>
       </c>
     </row>
     <row r="59" spans="1:18">
@@ -28819,7 +28806,7 @@
       </c>
       <c r="K59" s="31"/>
       <c r="L59" s="31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M59" s="31">
         <v>1E-3</v>
@@ -28831,10 +28818,10 @@
         <v>0.1</v>
       </c>
       <c r="P59" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="R59" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60" spans="1:18">
@@ -28864,7 +28851,7 @@
       </c>
       <c r="K60" s="31"/>
       <c r="L60" s="31">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M60" s="31">
         <v>1E-3</v>
@@ -28876,10 +28863,10 @@
         <v>0.1</v>
       </c>
       <c r="P60" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R60" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="61" spans="1:18">
@@ -28909,7 +28896,7 @@
       </c>
       <c r="K61" s="31"/>
       <c r="L61" s="31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M61" s="31">
         <v>1E-3</v>
@@ -28921,62 +28908,60 @@
         <v>0.1</v>
       </c>
       <c r="P61" t="s">
+        <v>144</v>
+      </c>
+      <c r="R61" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18">
+      <c r="C62" s="31">
+        <v>100</v>
+      </c>
+      <c r="D62" s="31">
+        <v>35</v>
+      </c>
+      <c r="E62" s="31">
+        <v>0</v>
+      </c>
+      <c r="F62" s="31">
+        <v>10</v>
+      </c>
+      <c r="G62" s="31">
+        <v>64</v>
+      </c>
+      <c r="H62" s="31">
+        <v>64</v>
+      </c>
+      <c r="I62" s="31">
+        <v>0</v>
+      </c>
+      <c r="J62" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K62" s="31"/>
+      <c r="L62" s="31">
+        <v>3</v>
+      </c>
+      <c r="M62" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N62" s="31">
+        <v>10</v>
+      </c>
+      <c r="O62" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P62" t="s">
         <v>143</v>
       </c>
-      <c r="R61" s="31">
+      <c r="R62" s="31">
         <v>57.424432000000003</v>
       </c>
     </row>
-    <row r="63" spans="1:18">
-      <c r="A63" t="s">
+    <row r="64" spans="1:18">
+      <c r="A64" t="s">
         <v>267</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18">
-      <c r="C64" s="31">
-        <v>100</v>
-      </c>
-      <c r="D64" s="31">
-        <v>35</v>
-      </c>
-      <c r="E64" s="31">
-        <v>0</v>
-      </c>
-      <c r="F64" s="31">
-        <v>10</v>
-      </c>
-      <c r="G64" s="31">
-        <v>32</v>
-      </c>
-      <c r="H64" s="31">
-        <v>64</v>
-      </c>
-      <c r="I64" s="31">
-        <v>0</v>
-      </c>
-      <c r="J64" s="31" t="s">
-        <v>148</v>
-      </c>
-      <c r="K64" s="31">
-        <v>1</v>
-      </c>
-      <c r="L64" s="31">
-        <v>1</v>
-      </c>
-      <c r="M64" s="31">
-        <v>1E-3</v>
-      </c>
-      <c r="N64" s="31">
-        <v>10</v>
-      </c>
-      <c r="O64" s="31">
-        <v>0.1</v>
-      </c>
-      <c r="P64" t="s">
-        <v>149</v>
-      </c>
-      <c r="R64" s="31">
-        <v>18.0412</v>
       </c>
     </row>
     <row r="65" spans="1:18">
@@ -29002,11 +28987,13 @@
         <v>0</v>
       </c>
       <c r="J65" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="K65" s="31"/>
+        <v>148</v>
+      </c>
+      <c r="K65" s="31">
+        <v>1</v>
+      </c>
       <c r="L65" s="31">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M65" s="31">
         <v>1E-3</v>
@@ -29018,10 +29005,10 @@
         <v>0.1</v>
       </c>
       <c r="P65" t="s">
-        <v>142</v>
-      </c>
-      <c r="R65" t="s">
-        <v>152</v>
+        <v>149</v>
+      </c>
+      <c r="R65" s="31">
+        <v>18.0412</v>
       </c>
     </row>
     <row r="66" spans="1:18">
@@ -29051,7 +29038,7 @@
       </c>
       <c r="K66" s="31"/>
       <c r="L66" s="31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M66" s="31">
         <v>1E-3</v>
@@ -29063,10 +29050,10 @@
         <v>0.1</v>
       </c>
       <c r="P66" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="R66" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="67" spans="1:18">
@@ -29096,7 +29083,7 @@
       </c>
       <c r="K67" s="31"/>
       <c r="L67" s="31">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M67" s="31">
         <v>1E-3</v>
@@ -29108,10 +29095,10 @@
         <v>0.1</v>
       </c>
       <c r="P67" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R67" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="68" spans="1:18">
@@ -29141,7 +29128,7 @@
       </c>
       <c r="K68" s="31"/>
       <c r="L68" s="31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M68" s="31">
         <v>1E-3</v>
@@ -29153,62 +29140,60 @@
         <v>0.1</v>
       </c>
       <c r="P68" t="s">
+        <v>144</v>
+      </c>
+      <c r="R68" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18">
+      <c r="C69" s="31">
+        <v>100</v>
+      </c>
+      <c r="D69" s="31">
+        <v>35</v>
+      </c>
+      <c r="E69" s="31">
+        <v>0</v>
+      </c>
+      <c r="F69" s="31">
+        <v>10</v>
+      </c>
+      <c r="G69" s="31">
+        <v>32</v>
+      </c>
+      <c r="H69" s="31">
+        <v>64</v>
+      </c>
+      <c r="I69" s="31">
+        <v>0</v>
+      </c>
+      <c r="J69" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K69" s="31"/>
+      <c r="L69" s="31">
+        <v>3</v>
+      </c>
+      <c r="M69" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N69" s="31">
+        <v>10</v>
+      </c>
+      <c r="O69" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P69" t="s">
         <v>143</v>
       </c>
-      <c r="R68" s="31">
+      <c r="R69" s="31">
         <v>57.424432000000003</v>
       </c>
     </row>
-    <row r="70" spans="1:18">
-      <c r="A70" t="s">
+    <row r="71" spans="1:18">
+      <c r="A71" t="s">
         <v>268</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18">
-      <c r="C71" s="31">
-        <v>100</v>
-      </c>
-      <c r="D71" s="31">
-        <v>35</v>
-      </c>
-      <c r="E71" s="31">
-        <v>0</v>
-      </c>
-      <c r="F71" s="31">
-        <v>10</v>
-      </c>
-      <c r="G71" s="31">
-        <v>16</v>
-      </c>
-      <c r="H71" s="31">
-        <v>64</v>
-      </c>
-      <c r="I71" s="31">
-        <v>0</v>
-      </c>
-      <c r="J71" s="31" t="s">
-        <v>148</v>
-      </c>
-      <c r="K71" s="31">
-        <v>1</v>
-      </c>
-      <c r="L71" s="31">
-        <v>1</v>
-      </c>
-      <c r="M71" s="31">
-        <v>1E-3</v>
-      </c>
-      <c r="N71" s="31">
-        <v>10</v>
-      </c>
-      <c r="O71" s="31">
-        <v>0.1</v>
-      </c>
-      <c r="P71" t="s">
-        <v>149</v>
-      </c>
-      <c r="R71" s="31">
-        <v>18.0412</v>
       </c>
     </row>
     <row r="72" spans="1:18">
@@ -29234,11 +29219,13 @@
         <v>0</v>
       </c>
       <c r="J72" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="K72" s="31"/>
+        <v>148</v>
+      </c>
+      <c r="K72" s="31">
+        <v>1</v>
+      </c>
       <c r="L72" s="31">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M72" s="31">
         <v>1E-3</v>
@@ -29250,10 +29237,10 @@
         <v>0.1</v>
       </c>
       <c r="P72" t="s">
-        <v>142</v>
-      </c>
-      <c r="R72" t="s">
-        <v>152</v>
+        <v>149</v>
+      </c>
+      <c r="R72" s="31">
+        <v>18.0412</v>
       </c>
     </row>
     <row r="73" spans="1:18">
@@ -29283,7 +29270,7 @@
       </c>
       <c r="K73" s="31"/>
       <c r="L73" s="31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M73" s="31">
         <v>1E-3</v>
@@ -29295,10 +29282,10 @@
         <v>0.1</v>
       </c>
       <c r="P73" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="R73" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="74" spans="1:18">
@@ -29328,7 +29315,7 @@
       </c>
       <c r="K74" s="31"/>
       <c r="L74" s="31">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M74" s="31">
         <v>1E-3</v>
@@ -29340,10 +29327,10 @@
         <v>0.1</v>
       </c>
       <c r="P74" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="R74" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="75" spans="1:18">
@@ -29373,7 +29360,7 @@
       </c>
       <c r="K75" s="31"/>
       <c r="L75" s="31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M75" s="31">
         <v>1E-3</v>
@@ -29385,474 +29372,1271 @@
         <v>0.1</v>
       </c>
       <c r="P75" t="s">
+        <v>144</v>
+      </c>
+      <c r="R75" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18">
+      <c r="C76" s="31">
+        <v>100</v>
+      </c>
+      <c r="D76" s="31">
+        <v>35</v>
+      </c>
+      <c r="E76" s="31">
+        <v>0</v>
+      </c>
+      <c r="F76" s="31">
+        <v>10</v>
+      </c>
+      <c r="G76" s="31">
+        <v>16</v>
+      </c>
+      <c r="H76" s="31">
+        <v>64</v>
+      </c>
+      <c r="I76" s="31">
+        <v>0</v>
+      </c>
+      <c r="J76" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="K76" s="31"/>
+      <c r="L76" s="31">
+        <v>3</v>
+      </c>
+      <c r="M76" s="31">
+        <v>1E-3</v>
+      </c>
+      <c r="N76" s="31">
+        <v>10</v>
+      </c>
+      <c r="O76" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="P76" t="s">
         <v>143</v>
       </c>
-      <c r="R75" s="31">
+      <c r="R76" s="31">
         <v>57.424432000000003</v>
       </c>
     </row>
     <row r="77" spans="1:18">
-      <c r="A77" t="s">
+      <c r="C77" s="31"/>
+      <c r="D77" s="31"/>
+      <c r="E77" s="31"/>
+      <c r="F77" s="31"/>
+      <c r="G77" s="31"/>
+      <c r="H77" s="31"/>
+      <c r="I77" s="31"/>
+      <c r="J77" s="31"/>
+      <c r="K77" s="31"/>
+      <c r="L77" s="31"/>
+      <c r="M77" s="31"/>
+      <c r="N77" s="31"/>
+      <c r="O77" s="31"/>
+      <c r="R77" s="31"/>
+    </row>
+    <row r="78" spans="1:18" s="16" customFormat="1">
+      <c r="A78" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="B78" s="27"/>
+      <c r="C78" s="53"/>
+      <c r="D78" s="53"/>
+      <c r="E78" s="53"/>
+      <c r="F78" s="53"/>
+      <c r="G78" s="53"/>
+      <c r="H78" s="53"/>
+      <c r="I78" s="53"/>
+      <c r="J78" s="53"/>
+      <c r="K78" s="53"/>
+      <c r="L78" s="53"/>
+      <c r="M78" s="53"/>
+      <c r="N78" s="53"/>
+      <c r="O78" s="53"/>
+      <c r="R78" s="53"/>
+    </row>
+    <row r="79" spans="1:18" s="16" customFormat="1">
+      <c r="B79" s="27">
+        <v>1406911</v>
+      </c>
+      <c r="C79" s="53">
+        <v>100</v>
+      </c>
+      <c r="D79" s="53">
+        <v>35</v>
+      </c>
+      <c r="E79" s="53">
+        <v>0</v>
+      </c>
+      <c r="F79" s="53">
+        <v>15</v>
+      </c>
+      <c r="G79" s="53">
+        <v>384</v>
+      </c>
+      <c r="H79" s="53">
+        <v>64</v>
+      </c>
+      <c r="I79" s="53">
+        <v>0</v>
+      </c>
+      <c r="J79" s="53" t="s">
+        <v>148</v>
+      </c>
+      <c r="K79" s="53">
+        <v>1</v>
+      </c>
+      <c r="L79" s="53">
+        <v>1</v>
+      </c>
+      <c r="M79" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N79" s="53">
+        <v>10</v>
+      </c>
+      <c r="O79" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="P79" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q79" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="R79" s="53">
+        <v>18.0412</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" s="16" customFormat="1">
+      <c r="B80" s="27">
+        <v>1406913</v>
+      </c>
+      <c r="C80" s="53">
+        <v>100</v>
+      </c>
+      <c r="D80" s="53">
+        <v>35</v>
+      </c>
+      <c r="E80" s="53">
+        <v>0</v>
+      </c>
+      <c r="F80" s="53">
+        <v>15</v>
+      </c>
+      <c r="G80" s="53">
+        <v>384</v>
+      </c>
+      <c r="H80" s="53">
+        <v>64</v>
+      </c>
+      <c r="I80" s="53">
+        <v>0</v>
+      </c>
+      <c r="J80" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K80" s="53"/>
+      <c r="L80" s="53">
+        <v>5</v>
+      </c>
+      <c r="M80" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N80" s="53">
+        <v>10</v>
+      </c>
+      <c r="O80" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="P80" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q80" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="R80" s="16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" s="16" customFormat="1">
+      <c r="B81" s="27">
+        <v>1406914</v>
+      </c>
+      <c r="C81" s="53">
+        <v>100</v>
+      </c>
+      <c r="D81" s="53">
+        <v>35</v>
+      </c>
+      <c r="E81" s="53">
+        <v>0</v>
+      </c>
+      <c r="F81" s="53">
+        <v>15</v>
+      </c>
+      <c r="G81" s="53">
+        <v>384</v>
+      </c>
+      <c r="H81" s="53">
+        <v>64</v>
+      </c>
+      <c r="I81" s="53">
+        <v>0</v>
+      </c>
+      <c r="J81" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K81" s="53"/>
+      <c r="L81" s="53">
+        <v>1</v>
+      </c>
+      <c r="M81" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N81" s="53">
+        <v>10</v>
+      </c>
+      <c r="O81" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="P81" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q81" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="R81" s="16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" s="16" customFormat="1">
+      <c r="B82" s="27">
+        <v>1406916</v>
+      </c>
+      <c r="C82" s="53">
+        <v>100</v>
+      </c>
+      <c r="D82" s="53">
+        <v>35</v>
+      </c>
+      <c r="E82" s="53">
+        <v>0</v>
+      </c>
+      <c r="F82" s="53">
+        <v>15</v>
+      </c>
+      <c r="G82" s="53">
+        <v>384</v>
+      </c>
+      <c r="H82" s="53">
+        <v>64</v>
+      </c>
+      <c r="I82" s="53">
+        <v>0</v>
+      </c>
+      <c r="J82" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K82" s="53"/>
+      <c r="L82" s="53">
+        <v>4</v>
+      </c>
+      <c r="M82" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N82" s="53">
+        <v>10</v>
+      </c>
+      <c r="O82" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="P82" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q82" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="R82" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" s="16" customFormat="1">
+      <c r="B83" s="27">
+        <v>1406921</v>
+      </c>
+      <c r="C83" s="53">
+        <v>100</v>
+      </c>
+      <c r="D83" s="53">
+        <v>35</v>
+      </c>
+      <c r="E83" s="53">
+        <v>0</v>
+      </c>
+      <c r="F83" s="53">
+        <v>15</v>
+      </c>
+      <c r="G83" s="53">
+        <v>384</v>
+      </c>
+      <c r="H83" s="53">
+        <v>64</v>
+      </c>
+      <c r="I83" s="53">
+        <v>0</v>
+      </c>
+      <c r="J83" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K83" s="53"/>
+      <c r="L83" s="53">
+        <v>3</v>
+      </c>
+      <c r="M83" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N83" s="53">
+        <v>10</v>
+      </c>
+      <c r="O83" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="P83" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q83" s="16">
+        <v>74</v>
+      </c>
+      <c r="R83" s="53">
+        <v>57.424432000000003</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" s="16" customFormat="1">
+      <c r="B84" s="27">
+        <v>1406923</v>
+      </c>
+      <c r="C84" s="53">
+        <v>100</v>
+      </c>
+      <c r="D84" s="53">
+        <v>35</v>
+      </c>
+      <c r="E84" s="53">
+        <v>0</v>
+      </c>
+      <c r="F84" s="53">
+        <v>15</v>
+      </c>
+      <c r="G84" s="53">
+        <v>384</v>
+      </c>
+      <c r="H84" s="53">
+        <v>64</v>
+      </c>
+      <c r="I84" s="53">
+        <v>0</v>
+      </c>
+      <c r="J84" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K84" s="53"/>
+      <c r="L84" s="53">
+        <v>0</v>
+      </c>
+      <c r="M84" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N84" s="53">
+        <v>10</v>
+      </c>
+      <c r="O84" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="P84" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="R84" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" s="16" customFormat="1">
+      <c r="B85" s="27"/>
+    </row>
+    <row r="86" spans="1:18" s="16" customFormat="1">
+      <c r="A86" s="16" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="78" spans="1:18">
-      <c r="C78" s="31">
+      <c r="B86" s="27"/>
+    </row>
+    <row r="87" spans="1:18" s="16" customFormat="1">
+      <c r="B87" s="27"/>
+      <c r="C87" s="53">
         <v>100</v>
       </c>
-      <c r="D78" s="31">
+      <c r="D87" s="53">
         <v>35</v>
       </c>
-      <c r="E78" s="31">
-        <v>0</v>
-      </c>
-      <c r="F78" s="31">
+      <c r="E87" s="53">
+        <v>0</v>
+      </c>
+      <c r="F87" s="53">
         <v>20</v>
       </c>
-      <c r="G78" s="31">
+      <c r="G87" s="53">
         <v>512</v>
       </c>
-      <c r="H78" s="31">
+      <c r="H87" s="53">
         <v>64</v>
       </c>
-      <c r="I78" s="31">
-        <v>0</v>
-      </c>
-      <c r="J78" s="31" t="s">
+      <c r="I87" s="53">
+        <v>0</v>
+      </c>
+      <c r="J87" s="53" t="s">
         <v>148</v>
       </c>
-      <c r="K78" s="31">
-        <v>1</v>
-      </c>
-      <c r="L78" s="31">
-        <v>1</v>
-      </c>
-      <c r="M78" s="31">
-        <v>1E-3</v>
-      </c>
-      <c r="N78" s="31">
-        <v>10</v>
-      </c>
-      <c r="O78" s="31">
+      <c r="K87" s="53">
+        <v>1</v>
+      </c>
+      <c r="L87" s="53">
+        <v>1</v>
+      </c>
+      <c r="M87" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N87" s="53">
+        <v>10</v>
+      </c>
+      <c r="O87" s="53">
         <v>0.1</v>
       </c>
-      <c r="P78" t="s">
+      <c r="P87" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="R78" s="31">
+      <c r="R87" s="53">
         <v>18.0412</v>
       </c>
     </row>
-    <row r="79" spans="1:18">
-      <c r="C79" s="31">
+    <row r="88" spans="1:18" s="16" customFormat="1">
+      <c r="B88" s="27"/>
+      <c r="C88" s="53">
         <v>100</v>
       </c>
-      <c r="D79" s="31">
+      <c r="D88" s="53">
         <v>35</v>
       </c>
-      <c r="E79" s="31">
-        <v>0</v>
-      </c>
-      <c r="F79" s="31">
+      <c r="E88" s="53">
+        <v>0</v>
+      </c>
+      <c r="F88" s="53">
         <v>20</v>
       </c>
-      <c r="G79" s="31">
+      <c r="G88" s="53">
         <v>512</v>
       </c>
-      <c r="H79" s="31">
+      <c r="H88" s="53">
         <v>64</v>
       </c>
-      <c r="I79" s="31">
-        <v>0</v>
-      </c>
-      <c r="J79" s="31" t="s">
+      <c r="I88" s="53">
+        <v>0</v>
+      </c>
+      <c r="J88" s="53" t="s">
         <v>146</v>
       </c>
-      <c r="K79" s="31"/>
-      <c r="L79" s="31">
+      <c r="K88" s="53"/>
+      <c r="L88" s="53">
         <v>5</v>
       </c>
-      <c r="M79" s="31">
-        <v>1E-3</v>
-      </c>
-      <c r="N79" s="31">
-        <v>10</v>
-      </c>
-      <c r="O79" s="31">
+      <c r="M88" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N88" s="53">
+        <v>10</v>
+      </c>
+      <c r="O88" s="53">
         <v>0.1</v>
       </c>
-      <c r="P79" t="s">
+      <c r="P88" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="R79" t="s">
+      <c r="R88" s="16" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="80" spans="1:18">
-      <c r="C80" s="31">
+    <row r="89" spans="1:18" s="16" customFormat="1">
+      <c r="B89" s="27"/>
+      <c r="C89" s="53">
         <v>100</v>
       </c>
-      <c r="D80" s="31">
+      <c r="D89" s="53">
         <v>35</v>
       </c>
-      <c r="E80" s="31">
-        <v>0</v>
-      </c>
-      <c r="F80" s="31">
+      <c r="E89" s="53">
+        <v>0</v>
+      </c>
+      <c r="F89" s="53">
         <v>20</v>
       </c>
-      <c r="G80" s="31">
+      <c r="G89" s="53">
         <v>512</v>
       </c>
-      <c r="H80" s="31">
+      <c r="H89" s="53">
         <v>64</v>
       </c>
-      <c r="I80" s="31">
-        <v>0</v>
-      </c>
-      <c r="J80" s="31" t="s">
+      <c r="I89" s="53">
+        <v>0</v>
+      </c>
+      <c r="J89" s="53" t="s">
         <v>146</v>
       </c>
-      <c r="K80" s="31"/>
-      <c r="L80" s="31">
-        <v>1</v>
-      </c>
-      <c r="M80" s="31">
-        <v>1E-3</v>
-      </c>
-      <c r="N80" s="31">
-        <v>10</v>
-      </c>
-      <c r="O80" s="31">
+      <c r="K89" s="53"/>
+      <c r="L89" s="53">
+        <v>1</v>
+      </c>
+      <c r="M89" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N89" s="53">
+        <v>10</v>
+      </c>
+      <c r="O89" s="53">
         <v>0.1</v>
       </c>
-      <c r="P80" t="s">
+      <c r="P89" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="R80" t="s">
+      <c r="R89" s="16" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="81" spans="1:18">
-      <c r="C81" s="31">
+    <row r="90" spans="1:18" s="16" customFormat="1">
+      <c r="B90" s="27"/>
+      <c r="C90" s="53">
         <v>100</v>
       </c>
-      <c r="D81" s="31">
+      <c r="D90" s="53">
         <v>35</v>
       </c>
-      <c r="E81" s="31">
-        <v>0</v>
-      </c>
-      <c r="F81" s="31">
+      <c r="E90" s="53">
+        <v>0</v>
+      </c>
+      <c r="F90" s="53">
         <v>20</v>
       </c>
-      <c r="G81" s="31">
+      <c r="G90" s="53">
         <v>512</v>
       </c>
-      <c r="H81" s="31">
+      <c r="H90" s="53">
         <v>64</v>
       </c>
-      <c r="I81" s="31">
-        <v>0</v>
-      </c>
-      <c r="J81" s="31" t="s">
+      <c r="I90" s="53">
+        <v>0</v>
+      </c>
+      <c r="J90" s="53" t="s">
         <v>146</v>
       </c>
-      <c r="K81" s="31"/>
-      <c r="L81" s="31">
+      <c r="K90" s="53"/>
+      <c r="L90" s="53">
         <v>4</v>
       </c>
-      <c r="M81" s="31">
-        <v>1E-3</v>
-      </c>
-      <c r="N81" s="31">
-        <v>10</v>
-      </c>
-      <c r="O81" s="31">
+      <c r="M90" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N90" s="53">
+        <v>10</v>
+      </c>
+      <c r="O90" s="53">
         <v>0.1</v>
       </c>
-      <c r="P81" t="s">
+      <c r="P90" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="R81" t="s">
+      <c r="R90" s="16" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="82" spans="1:18">
-      <c r="C82" s="31">
+    <row r="91" spans="1:18" s="16" customFormat="1">
+      <c r="B91" s="27"/>
+      <c r="C91" s="53">
         <v>100</v>
       </c>
-      <c r="D82" s="31">
+      <c r="D91" s="53">
         <v>35</v>
       </c>
-      <c r="E82" s="31">
-        <v>0</v>
-      </c>
-      <c r="F82" s="31">
+      <c r="E91" s="53">
+        <v>0</v>
+      </c>
+      <c r="F91" s="53">
         <v>20</v>
       </c>
-      <c r="G82" s="31">
+      <c r="G91" s="53">
         <v>512</v>
       </c>
-      <c r="H82" s="31">
+      <c r="H91" s="53">
         <v>64</v>
       </c>
-      <c r="I82" s="31">
-        <v>0</v>
-      </c>
-      <c r="J82" s="31" t="s">
+      <c r="I91" s="53">
+        <v>0</v>
+      </c>
+      <c r="J91" s="53" t="s">
         <v>146</v>
       </c>
-      <c r="K82" s="31"/>
-      <c r="L82" s="31">
+      <c r="K91" s="53"/>
+      <c r="L91" s="53">
         <v>3</v>
       </c>
-      <c r="M82" s="31">
-        <v>1E-3</v>
-      </c>
-      <c r="N82" s="31">
-        <v>10</v>
-      </c>
-      <c r="O82" s="31">
+      <c r="M91" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N91" s="53">
+        <v>10</v>
+      </c>
+      <c r="O91" s="53">
         <v>0.1</v>
       </c>
-      <c r="P82" t="s">
+      <c r="P91" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="R82" s="31">
+      <c r="R91" s="53">
         <v>57.424432000000003</v>
       </c>
     </row>
-    <row r="84" spans="1:18">
-      <c r="A84" t="s">
+    <row r="92" spans="1:18" s="16" customFormat="1">
+      <c r="B92" s="27"/>
+      <c r="C92" s="53">
+        <v>100</v>
+      </c>
+      <c r="D92" s="53">
+        <v>35</v>
+      </c>
+      <c r="E92" s="53">
+        <v>0</v>
+      </c>
+      <c r="F92" s="53">
+        <v>20</v>
+      </c>
+      <c r="G92" s="53">
+        <v>512</v>
+      </c>
+      <c r="H92" s="53">
+        <v>64</v>
+      </c>
+      <c r="I92" s="53">
+        <v>0</v>
+      </c>
+      <c r="J92" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K92" s="53"/>
+      <c r="L92" s="53">
+        <v>0</v>
+      </c>
+      <c r="M92" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N92" s="53">
+        <v>10</v>
+      </c>
+      <c r="O92" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="P92" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="R92" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" s="16" customFormat="1">
+      <c r="B93" s="27"/>
+      <c r="C93" s="53"/>
+      <c r="D93" s="53"/>
+      <c r="E93" s="53"/>
+      <c r="F93" s="53"/>
+      <c r="G93" s="53"/>
+      <c r="H93" s="53"/>
+      <c r="I93" s="53"/>
+      <c r="J93" s="53"/>
+      <c r="K93" s="53"/>
+      <c r="L93" s="53"/>
+      <c r="M93" s="53"/>
+      <c r="N93" s="53"/>
+      <c r="O93" s="53"/>
+      <c r="R93" s="53"/>
+    </row>
+    <row r="94" spans="1:18" s="16" customFormat="1">
+      <c r="A94" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="B94" s="27"/>
+    </row>
+    <row r="95" spans="1:18" s="16" customFormat="1">
+      <c r="B95" s="27"/>
+      <c r="C95" s="53">
+        <v>100</v>
+      </c>
+      <c r="D95" s="53">
+        <v>35</v>
+      </c>
+      <c r="E95" s="53">
+        <v>0</v>
+      </c>
+      <c r="F95" s="53">
+        <v>30</v>
+      </c>
+      <c r="G95" s="53">
+        <v>768</v>
+      </c>
+      <c r="H95" s="53">
+        <v>64</v>
+      </c>
+      <c r="I95" s="53">
+        <v>0</v>
+      </c>
+      <c r="J95" s="53" t="s">
+        <v>148</v>
+      </c>
+      <c r="K95" s="53">
+        <v>1</v>
+      </c>
+      <c r="L95" s="53">
+        <v>1</v>
+      </c>
+      <c r="M95" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N95" s="53">
+        <v>10</v>
+      </c>
+      <c r="O95" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="P95" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="R95" s="53">
+        <v>18.0412</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" s="16" customFormat="1">
+      <c r="B96" s="27"/>
+      <c r="C96" s="53">
+        <v>100</v>
+      </c>
+      <c r="D96" s="53">
+        <v>35</v>
+      </c>
+      <c r="E96" s="53">
+        <v>0</v>
+      </c>
+      <c r="F96" s="53">
+        <v>30</v>
+      </c>
+      <c r="G96" s="53">
+        <v>768</v>
+      </c>
+      <c r="H96" s="53">
+        <v>64</v>
+      </c>
+      <c r="I96" s="53">
+        <v>0</v>
+      </c>
+      <c r="J96" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K96" s="53"/>
+      <c r="L96" s="53">
+        <v>5</v>
+      </c>
+      <c r="M96" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N96" s="53">
+        <v>10</v>
+      </c>
+      <c r="O96" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="P96" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="R96" s="16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="97" spans="1:18" s="16" customFormat="1">
+      <c r="B97" s="27"/>
+      <c r="C97" s="53">
+        <v>100</v>
+      </c>
+      <c r="D97" s="53">
+        <v>35</v>
+      </c>
+      <c r="E97" s="53">
+        <v>0</v>
+      </c>
+      <c r="F97" s="53">
+        <v>30</v>
+      </c>
+      <c r="G97" s="53">
+        <v>768</v>
+      </c>
+      <c r="H97" s="53">
+        <v>64</v>
+      </c>
+      <c r="I97" s="53">
+        <v>0</v>
+      </c>
+      <c r="J97" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K97" s="53"/>
+      <c r="L97" s="53">
+        <v>1</v>
+      </c>
+      <c r="M97" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N97" s="53">
+        <v>10</v>
+      </c>
+      <c r="O97" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="P97" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="R97" s="16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18" s="16" customFormat="1">
+      <c r="B98" s="27"/>
+      <c r="C98" s="53">
+        <v>100</v>
+      </c>
+      <c r="D98" s="53">
+        <v>35</v>
+      </c>
+      <c r="E98" s="53">
+        <v>0</v>
+      </c>
+      <c r="F98" s="53">
+        <v>30</v>
+      </c>
+      <c r="G98" s="53">
+        <v>768</v>
+      </c>
+      <c r="H98" s="53">
+        <v>64</v>
+      </c>
+      <c r="I98" s="53">
+        <v>0</v>
+      </c>
+      <c r="J98" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K98" s="53"/>
+      <c r="L98" s="53">
+        <v>4</v>
+      </c>
+      <c r="M98" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N98" s="53">
+        <v>10</v>
+      </c>
+      <c r="O98" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="P98" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="R98" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" s="16" customFormat="1">
+      <c r="B99" s="27"/>
+      <c r="C99" s="53">
+        <v>100</v>
+      </c>
+      <c r="D99" s="53">
+        <v>35</v>
+      </c>
+      <c r="E99" s="53">
+        <v>0</v>
+      </c>
+      <c r="F99" s="53">
+        <v>30</v>
+      </c>
+      <c r="G99" s="53">
+        <v>768</v>
+      </c>
+      <c r="H99" s="53">
+        <v>64</v>
+      </c>
+      <c r="I99" s="53">
+        <v>0</v>
+      </c>
+      <c r="J99" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K99" s="53"/>
+      <c r="L99" s="53">
+        <v>3</v>
+      </c>
+      <c r="M99" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N99" s="53">
+        <v>10</v>
+      </c>
+      <c r="O99" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="P99" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="R99" s="53">
+        <v>57.424432000000003</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" s="16" customFormat="1">
+      <c r="B100" s="27"/>
+      <c r="C100" s="53">
+        <v>100</v>
+      </c>
+      <c r="D100" s="53">
+        <v>35</v>
+      </c>
+      <c r="E100" s="53">
+        <v>0</v>
+      </c>
+      <c r="F100" s="53">
+        <v>30</v>
+      </c>
+      <c r="G100" s="53">
+        <v>768</v>
+      </c>
+      <c r="H100" s="53">
+        <v>64</v>
+      </c>
+      <c r="I100" s="53">
+        <v>0</v>
+      </c>
+      <c r="J100" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K100" s="53"/>
+      <c r="L100" s="53">
+        <v>0</v>
+      </c>
+      <c r="M100" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N100" s="53">
+        <v>10</v>
+      </c>
+      <c r="O100" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="P100" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="R100" s="53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" s="16" customFormat="1">
+      <c r="B101" s="27"/>
+    </row>
+    <row r="102" spans="1:18" s="16" customFormat="1">
+      <c r="A102" s="16" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="85" spans="1:18">
-      <c r="C85" s="31">
+      <c r="B102" s="27"/>
+    </row>
+    <row r="103" spans="1:18" s="16" customFormat="1">
+      <c r="B103" s="27"/>
+      <c r="C103" s="53">
         <v>100</v>
       </c>
-      <c r="D85" s="31">
+      <c r="D103" s="53">
         <v>35</v>
       </c>
-      <c r="E85" s="31">
-        <v>0</v>
-      </c>
-      <c r="F85" s="31">
+      <c r="E103" s="53">
+        <v>0</v>
+      </c>
+      <c r="F103" s="53">
         <v>40</v>
       </c>
-      <c r="G85" s="31">
+      <c r="G103" s="53">
         <v>1024</v>
       </c>
-      <c r="H85" s="31">
+      <c r="H103" s="53">
         <v>64</v>
       </c>
-      <c r="I85" s="31">
-        <v>0</v>
-      </c>
-      <c r="J85" s="31" t="s">
+      <c r="I103" s="53">
+        <v>0</v>
+      </c>
+      <c r="J103" s="53" t="s">
         <v>148</v>
       </c>
-      <c r="K85" s="31">
-        <v>1</v>
-      </c>
-      <c r="L85" s="31">
-        <v>1</v>
-      </c>
-      <c r="M85" s="31">
-        <v>1E-3</v>
-      </c>
-      <c r="N85" s="31">
-        <v>10</v>
-      </c>
-      <c r="O85" s="31">
+      <c r="K103" s="53">
+        <v>1</v>
+      </c>
+      <c r="L103" s="53">
+        <v>1</v>
+      </c>
+      <c r="M103" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N103" s="53">
+        <v>10</v>
+      </c>
+      <c r="O103" s="53">
         <v>0.1</v>
       </c>
-      <c r="P85" t="s">
+      <c r="P103" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="R85" s="31">
+      <c r="R103" s="53">
         <v>18.0412</v>
       </c>
     </row>
-    <row r="86" spans="1:18">
-      <c r="C86" s="31">
+    <row r="104" spans="1:18" s="16" customFormat="1">
+      <c r="B104" s="27"/>
+      <c r="C104" s="53">
         <v>100</v>
       </c>
-      <c r="D86" s="31">
+      <c r="D104" s="53">
         <v>35</v>
       </c>
-      <c r="E86" s="31">
-        <v>0</v>
-      </c>
-      <c r="F86" s="31">
+      <c r="E104" s="53">
+        <v>0</v>
+      </c>
+      <c r="F104" s="53">
         <v>40</v>
       </c>
-      <c r="G86" s="31">
+      <c r="G104" s="53">
         <v>1024</v>
       </c>
-      <c r="H86" s="31">
+      <c r="H104" s="53">
         <v>64</v>
       </c>
-      <c r="I86" s="31">
-        <v>0</v>
-      </c>
-      <c r="J86" s="31" t="s">
+      <c r="I104" s="53">
+        <v>0</v>
+      </c>
+      <c r="J104" s="53" t="s">
         <v>146</v>
       </c>
-      <c r="K86" s="31"/>
-      <c r="L86" s="31">
+      <c r="K104" s="53"/>
+      <c r="L104" s="53">
         <v>5</v>
       </c>
-      <c r="M86" s="31">
-        <v>1E-3</v>
-      </c>
-      <c r="N86" s="31">
-        <v>10</v>
-      </c>
-      <c r="O86" s="31">
+      <c r="M104" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N104" s="53">
+        <v>10</v>
+      </c>
+      <c r="O104" s="53">
         <v>0.1</v>
       </c>
-      <c r="P86" t="s">
+      <c r="P104" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="R86" t="s">
+      <c r="R104" s="16" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="87" spans="1:18">
-      <c r="C87" s="31">
+    <row r="105" spans="1:18" s="16" customFormat="1">
+      <c r="B105" s="27"/>
+      <c r="C105" s="53">
         <v>100</v>
       </c>
-      <c r="D87" s="31">
+      <c r="D105" s="53">
         <v>35</v>
       </c>
-      <c r="E87" s="31">
-        <v>0</v>
-      </c>
-      <c r="F87" s="31">
+      <c r="E105" s="53">
+        <v>0</v>
+      </c>
+      <c r="F105" s="53">
         <v>40</v>
       </c>
-      <c r="G87" s="31">
+      <c r="G105" s="53">
         <v>1024</v>
       </c>
-      <c r="H87" s="31">
+      <c r="H105" s="53">
         <v>64</v>
       </c>
-      <c r="I87" s="31">
-        <v>0</v>
-      </c>
-      <c r="J87" s="31" t="s">
+      <c r="I105" s="53">
+        <v>0</v>
+      </c>
+      <c r="J105" s="53" t="s">
         <v>146</v>
       </c>
-      <c r="K87" s="31"/>
-      <c r="L87" s="31">
-        <v>1</v>
-      </c>
-      <c r="M87" s="31">
-        <v>1E-3</v>
-      </c>
-      <c r="N87" s="31">
-        <v>10</v>
-      </c>
-      <c r="O87" s="31">
+      <c r="K105" s="53"/>
+      <c r="L105" s="53">
+        <v>1</v>
+      </c>
+      <c r="M105" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N105" s="53">
+        <v>10</v>
+      </c>
+      <c r="O105" s="53">
         <v>0.1</v>
       </c>
-      <c r="P87" t="s">
+      <c r="P105" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="R87" t="s">
+      <c r="R105" s="16" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="88" spans="1:18">
-      <c r="C88" s="31">
+    <row r="106" spans="1:18" s="16" customFormat="1">
+      <c r="B106" s="27"/>
+      <c r="C106" s="53">
         <v>100</v>
       </c>
-      <c r="D88" s="31">
+      <c r="D106" s="53">
         <v>35</v>
       </c>
-      <c r="E88" s="31">
-        <v>0</v>
-      </c>
-      <c r="F88" s="31">
+      <c r="E106" s="53">
+        <v>0</v>
+      </c>
+      <c r="F106" s="53">
         <v>40</v>
       </c>
-      <c r="G88" s="31">
+      <c r="G106" s="53">
         <v>1024</v>
       </c>
-      <c r="H88" s="31">
+      <c r="H106" s="53">
         <v>64</v>
       </c>
-      <c r="I88" s="31">
-        <v>0</v>
-      </c>
-      <c r="J88" s="31" t="s">
+      <c r="I106" s="53">
+        <v>0</v>
+      </c>
+      <c r="J106" s="53" t="s">
         <v>146</v>
       </c>
-      <c r="K88" s="31"/>
-      <c r="L88" s="31">
+      <c r="K106" s="53"/>
+      <c r="L106" s="53">
         <v>4</v>
       </c>
-      <c r="M88" s="31">
-        <v>1E-3</v>
-      </c>
-      <c r="N88" s="31">
-        <v>10</v>
-      </c>
-      <c r="O88" s="31">
+      <c r="M106" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N106" s="53">
+        <v>10</v>
+      </c>
+      <c r="O106" s="53">
         <v>0.1</v>
       </c>
-      <c r="P88" t="s">
+      <c r="P106" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="R88" t="s">
+      <c r="R106" s="16" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="89" spans="1:18">
-      <c r="C89" s="31">
+    <row r="107" spans="1:18" s="16" customFormat="1">
+      <c r="B107" s="27"/>
+      <c r="C107" s="53">
         <v>100</v>
       </c>
-      <c r="D89" s="31">
+      <c r="D107" s="53">
         <v>35</v>
       </c>
-      <c r="E89" s="31">
-        <v>0</v>
-      </c>
-      <c r="F89" s="31">
+      <c r="E107" s="53">
+        <v>0</v>
+      </c>
+      <c r="F107" s="53">
         <v>40</v>
       </c>
-      <c r="G89" s="31">
+      <c r="G107" s="53">
         <v>1024</v>
       </c>
-      <c r="H89" s="31">
+      <c r="H107" s="53">
         <v>64</v>
       </c>
-      <c r="I89" s="31">
-        <v>0</v>
-      </c>
-      <c r="J89" s="31" t="s">
+      <c r="I107" s="53">
+        <v>0</v>
+      </c>
+      <c r="J107" s="53" t="s">
         <v>146</v>
       </c>
-      <c r="K89" s="31"/>
-      <c r="L89" s="31">
+      <c r="K107" s="53"/>
+      <c r="L107" s="53">
         <v>3</v>
       </c>
-      <c r="M89" s="31">
-        <v>1E-3</v>
-      </c>
-      <c r="N89" s="31">
-        <v>10</v>
-      </c>
-      <c r="O89" s="31">
+      <c r="M107" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N107" s="53">
+        <v>10</v>
+      </c>
+      <c r="O107" s="53">
         <v>0.1</v>
       </c>
-      <c r="P89" t="s">
+      <c r="P107" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="R89" s="31">
+      <c r="R107" s="53">
         <v>57.424432000000003</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" s="16" customFormat="1">
+      <c r="B108" s="27"/>
+      <c r="C108" s="53">
+        <v>100</v>
+      </c>
+      <c r="D108" s="53">
+        <v>35</v>
+      </c>
+      <c r="E108" s="53">
+        <v>0</v>
+      </c>
+      <c r="F108" s="53">
+        <v>40</v>
+      </c>
+      <c r="G108" s="53">
+        <v>1024</v>
+      </c>
+      <c r="H108" s="53">
+        <v>64</v>
+      </c>
+      <c r="I108" s="53">
+        <v>0</v>
+      </c>
+      <c r="J108" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K108" s="53"/>
+      <c r="L108" s="53">
+        <v>0</v>
+      </c>
+      <c r="M108" s="53">
+        <v>1E-3</v>
+      </c>
+      <c r="N108" s="53">
+        <v>10</v>
+      </c>
+      <c r="O108" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="P108" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="R108" s="53">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 3D fixed flux RBC
</commit_message>
<xml_diff>
--- a/dedalus_case.xlsx
+++ b/dedalus_case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nutstore\Nutstore\Workspace\dedalus_main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411E0DE1-076B-41F7-B208-AF7A04571371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C899C317-EC8C-4A0F-ADAC-4D103C3938DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="602" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="602" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RBC flux" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1814" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1837" uniqueCount="316">
   <si>
     <t>slurm_num</t>
   </si>
@@ -1001,6 +1001,18 @@
   <si>
     <t>Lx=160,Nx=4096</t>
   </si>
+  <si>
+    <t>Updaate Revision 2 add high Ra cases!!! Uconn cluster</t>
+  </si>
+  <si>
+    <t>Chaotic state from 1e8</t>
+  </si>
+  <si>
+    <t>Elevator mode, 12 hours</t>
+  </si>
+  <si>
+    <t>Elevator mode, 150 hours</t>
+  </si>
 </sst>
 </file>
 
@@ -1121,7 +1133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1183,8 +1195,6 @@
     <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1465,10 +1475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S406"/>
+  <dimension ref="A1:S422"/>
   <sheetViews>
-    <sheetView topLeftCell="A399" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C406" sqref="C406:N406"/>
+    <sheetView tabSelected="1" topLeftCell="A408" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B410" sqref="B410"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -16199,6 +16209,523 @@
       </c>
       <c r="N406" s="8">
         <v>0.01</v>
+      </c>
+    </row>
+    <row r="408" spans="1:14">
+      <c r="A408" s="16" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="409" spans="1:14">
+      <c r="A409" t="s">
+        <v>313</v>
+      </c>
+      <c r="B409">
+        <v>4604162</v>
+      </c>
+      <c r="C409" s="2">
+        <v>300000000</v>
+      </c>
+      <c r="D409" s="8">
+        <v>1</v>
+      </c>
+      <c r="E409" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F409" s="8">
+        <v>1</v>
+      </c>
+      <c r="G409" s="8">
+        <v>512</v>
+      </c>
+      <c r="H409" s="8">
+        <v>512</v>
+      </c>
+      <c r="I409" s="8">
+        <v>10</v>
+      </c>
+      <c r="J409" s="8">
+        <v>10</v>
+      </c>
+      <c r="K409" s="8">
+        <v>0</v>
+      </c>
+      <c r="L409" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M409" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="N409" s="8">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="410" spans="1:14">
+      <c r="A410" t="s">
+        <v>313</v>
+      </c>
+      <c r="B410">
+        <v>4603634</v>
+      </c>
+      <c r="C410" s="2">
+        <v>300000000</v>
+      </c>
+      <c r="D410" s="8">
+        <v>1</v>
+      </c>
+      <c r="E410" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F410" s="8">
+        <v>1</v>
+      </c>
+      <c r="G410" s="8">
+        <v>512</v>
+      </c>
+      <c r="H410" s="8">
+        <v>512</v>
+      </c>
+      <c r="I410" s="8">
+        <v>10</v>
+      </c>
+      <c r="J410" s="8">
+        <v>10</v>
+      </c>
+      <c r="K410" s="8">
+        <v>0</v>
+      </c>
+      <c r="L410" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M410" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="N410" s="8">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="411" spans="1:14">
+      <c r="A411" t="s">
+        <v>313</v>
+      </c>
+      <c r="B411">
+        <v>4603681</v>
+      </c>
+      <c r="C411" s="2">
+        <v>1000000000</v>
+      </c>
+      <c r="D411" s="8">
+        <v>1</v>
+      </c>
+      <c r="E411" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F411" s="8">
+        <v>1</v>
+      </c>
+      <c r="G411" s="8">
+        <v>512</v>
+      </c>
+      <c r="H411" s="8">
+        <v>512</v>
+      </c>
+      <c r="I411" s="8">
+        <v>10</v>
+      </c>
+      <c r="J411" s="8">
+        <v>10</v>
+      </c>
+      <c r="K411" s="8">
+        <v>0</v>
+      </c>
+      <c r="L411" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M411" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="N411" s="8">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="412" spans="1:14">
+      <c r="A412" t="s">
+        <v>313</v>
+      </c>
+      <c r="B412">
+        <v>4603691</v>
+      </c>
+      <c r="C412" s="2">
+        <v>3000000000</v>
+      </c>
+      <c r="D412" s="8">
+        <v>1</v>
+      </c>
+      <c r="E412" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F412" s="8">
+        <v>1</v>
+      </c>
+      <c r="G412" s="8">
+        <v>512</v>
+      </c>
+      <c r="H412" s="8">
+        <v>512</v>
+      </c>
+      <c r="I412" s="8">
+        <v>10</v>
+      </c>
+      <c r="J412" s="8">
+        <v>10</v>
+      </c>
+      <c r="K412" s="8">
+        <v>0</v>
+      </c>
+      <c r="L412" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M412" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="N412" s="8">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="413" spans="1:14">
+      <c r="A413" t="s">
+        <v>313</v>
+      </c>
+      <c r="B413">
+        <v>4603698</v>
+      </c>
+      <c r="C413" s="2">
+        <v>10000000000</v>
+      </c>
+      <c r="D413" s="8">
+        <v>1</v>
+      </c>
+      <c r="E413" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F413" s="8">
+        <v>1</v>
+      </c>
+      <c r="G413" s="8">
+        <v>512</v>
+      </c>
+      <c r="H413" s="8">
+        <v>512</v>
+      </c>
+      <c r="I413" s="8">
+        <v>10</v>
+      </c>
+      <c r="J413" s="8">
+        <v>10</v>
+      </c>
+      <c r="K413" s="8">
+        <v>0</v>
+      </c>
+      <c r="L413" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M413" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="N413" s="8">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="414" spans="1:14">
+      <c r="C414" s="2"/>
+      <c r="D414" s="8"/>
+      <c r="E414" s="8"/>
+      <c r="F414" s="8"/>
+      <c r="G414" s="8"/>
+      <c r="H414" s="8"/>
+      <c r="I414" s="8"/>
+      <c r="J414" s="8"/>
+      <c r="K414" s="8"/>
+      <c r="L414" s="2"/>
+      <c r="M414" s="8"/>
+      <c r="N414" s="8"/>
+    </row>
+    <row r="415" spans="1:14">
+      <c r="C415" s="2"/>
+      <c r="D415" s="8"/>
+      <c r="E415" s="8"/>
+      <c r="F415" s="8"/>
+      <c r="G415" s="8"/>
+      <c r="H415" s="8"/>
+      <c r="I415" s="8"/>
+      <c r="J415" s="8"/>
+      <c r="K415" s="8"/>
+      <c r="L415" s="2"/>
+      <c r="M415" s="8"/>
+      <c r="N415" s="8"/>
+    </row>
+    <row r="416" spans="1:14">
+      <c r="A416" t="s">
+        <v>313</v>
+      </c>
+      <c r="B416">
+        <v>4603853</v>
+      </c>
+      <c r="C416" s="2">
+        <v>300000000</v>
+      </c>
+      <c r="D416" s="8">
+        <v>1</v>
+      </c>
+      <c r="E416" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="F416" s="8">
+        <v>1</v>
+      </c>
+      <c r="G416" s="8">
+        <v>512</v>
+      </c>
+      <c r="H416" s="8">
+        <v>512</v>
+      </c>
+      <c r="I416" s="8">
+        <v>10</v>
+      </c>
+      <c r="J416" s="8">
+        <v>10</v>
+      </c>
+      <c r="K416" s="8">
+        <v>0</v>
+      </c>
+      <c r="L416" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M416" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="N416" s="8">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="417" spans="1:14">
+      <c r="A417" t="s">
+        <v>313</v>
+      </c>
+      <c r="B417">
+        <v>4603881</v>
+      </c>
+      <c r="C417" s="2">
+        <v>1000000000</v>
+      </c>
+      <c r="D417" s="8">
+        <v>1</v>
+      </c>
+      <c r="E417" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="F417" s="8">
+        <v>1</v>
+      </c>
+      <c r="G417" s="8">
+        <v>512</v>
+      </c>
+      <c r="H417" s="8">
+        <v>512</v>
+      </c>
+      <c r="I417" s="8">
+        <v>10</v>
+      </c>
+      <c r="J417" s="8">
+        <v>10</v>
+      </c>
+      <c r="K417" s="8">
+        <v>0</v>
+      </c>
+      <c r="L417" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M417" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="N417" s="8">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="418" spans="1:14">
+      <c r="A418" t="s">
+        <v>313</v>
+      </c>
+      <c r="B418">
+        <v>4603901</v>
+      </c>
+      <c r="C418" s="2">
+        <v>3000000000</v>
+      </c>
+      <c r="D418" s="8">
+        <v>1</v>
+      </c>
+      <c r="E418" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="F418" s="8">
+        <v>1</v>
+      </c>
+      <c r="G418" s="8">
+        <v>512</v>
+      </c>
+      <c r="H418" s="8">
+        <v>512</v>
+      </c>
+      <c r="I418" s="8">
+        <v>10</v>
+      </c>
+      <c r="J418" s="8">
+        <v>10</v>
+      </c>
+      <c r="K418" s="8">
+        <v>0</v>
+      </c>
+      <c r="L418" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M418" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="N418" s="8">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="419" spans="1:14">
+      <c r="A419" t="s">
+        <v>313</v>
+      </c>
+      <c r="B419">
+        <v>4604079</v>
+      </c>
+      <c r="C419" s="2">
+        <v>10000000000</v>
+      </c>
+      <c r="D419" s="8">
+        <v>1</v>
+      </c>
+      <c r="E419" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="F419" s="8">
+        <v>1</v>
+      </c>
+      <c r="G419" s="8">
+        <v>512</v>
+      </c>
+      <c r="H419" s="8">
+        <v>512</v>
+      </c>
+      <c r="I419" s="8">
+        <v>10</v>
+      </c>
+      <c r="J419" s="8">
+        <v>10</v>
+      </c>
+      <c r="K419" s="8">
+        <v>0</v>
+      </c>
+      <c r="L419" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M419" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="N419" s="8">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="421" spans="1:14">
+      <c r="A421" t="s">
+        <v>314</v>
+      </c>
+      <c r="B421">
+        <v>4604145</v>
+      </c>
+      <c r="C421" s="2">
+        <v>10000000000</v>
+      </c>
+      <c r="D421" s="8">
+        <v>1</v>
+      </c>
+      <c r="E421" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F421" s="8">
+        <v>1</v>
+      </c>
+      <c r="G421" s="8">
+        <v>1024</v>
+      </c>
+      <c r="H421" s="8">
+        <v>1024</v>
+      </c>
+      <c r="I421" s="8">
+        <v>10</v>
+      </c>
+      <c r="J421" s="8">
+        <v>10</v>
+      </c>
+      <c r="K421" s="8">
+        <v>0</v>
+      </c>
+      <c r="L421" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M421" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="N421" s="8">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="422" spans="1:14">
+      <c r="A422" t="s">
+        <v>315</v>
+      </c>
+      <c r="B422">
+        <v>4604148</v>
+      </c>
+      <c r="C422" s="2">
+        <v>10000000000</v>
+      </c>
+      <c r="D422" s="8">
+        <v>1</v>
+      </c>
+      <c r="E422" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F422" s="8">
+        <v>1</v>
+      </c>
+      <c r="G422" s="8">
+        <v>1024</v>
+      </c>
+      <c r="H422" s="8">
+        <v>1024</v>
+      </c>
+      <c r="I422" s="8">
+        <v>10</v>
+      </c>
+      <c r="J422" s="8">
+        <v>10</v>
+      </c>
+      <c r="K422" s="8">
+        <v>0</v>
+      </c>
+      <c r="L422" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="M422" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="N422" s="8">
+        <v>1E-3</v>
       </c>
     </row>
   </sheetData>
@@ -26992,7 +27519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C73000ED-ACF1-4870-B376-DD86BAB5368D}">
   <dimension ref="A1:T160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A149" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B161" sqref="B161"/>
     </sheetView>
   </sheetViews>
@@ -32189,7 +32716,7 @@
       </c>
     </row>
     <row r="149" spans="1:20" s="16" customFormat="1">
-      <c r="B149" s="59">
+      <c r="B149" s="45">
         <v>2101202</v>
       </c>
       <c r="C149" s="53">
@@ -32281,7 +32808,7 @@
       </c>
     </row>
     <row r="151" spans="1:20" s="16" customFormat="1">
-      <c r="B151" s="60">
+      <c r="B151" s="27">
         <v>2101203</v>
       </c>
       <c r="C151" s="53">
@@ -32327,7 +32854,7 @@
       </c>
     </row>
     <row r="152" spans="1:20" s="16" customFormat="1">
-      <c r="B152" s="60">
+      <c r="B152" s="27">
         <v>2101205</v>
       </c>
       <c r="C152" s="53">
@@ -32373,7 +32900,7 @@
       </c>
     </row>
     <row r="153" spans="1:20" s="16" customFormat="1">
-      <c r="B153" s="60">
+      <c r="B153" s="27">
         <v>2101207</v>
       </c>
       <c r="C153" s="53">
@@ -32424,7 +32951,7 @@
       </c>
     </row>
     <row r="156" spans="1:20" s="16" customFormat="1">
-      <c r="B156" s="60">
+      <c r="B156" s="27">
         <v>2101210</v>
       </c>
       <c r="C156" s="53">
@@ -32470,7 +32997,7 @@
       </c>
     </row>
     <row r="157" spans="1:20" s="16" customFormat="1">
-      <c r="B157" s="60">
+      <c r="B157" s="27">
         <v>2101212</v>
       </c>
       <c r="C157" s="53">
@@ -32516,7 +33043,7 @@
       </c>
     </row>
     <row r="158" spans="1:20" s="16" customFormat="1">
-      <c r="B158" s="60">
+      <c r="B158" s="27">
         <v>2101216</v>
       </c>
       <c r="C158" s="53">
@@ -32562,7 +33089,7 @@
       </c>
     </row>
     <row r="159" spans="1:20" s="16" customFormat="1">
-      <c r="B159" s="60">
+      <c r="B159" s="27">
         <v>2102431</v>
       </c>
       <c r="C159" s="53">
@@ -32608,7 +33135,7 @@
       </c>
     </row>
     <row r="160" spans="1:20" s="16" customFormat="1">
-      <c r="B160" s="60">
+      <c r="B160" s="27">
         <v>2102432</v>
       </c>
       <c r="C160" s="53">

</xml_diff>